<commit_message>
Pipes, edits, boilers and lots more
</commit_message>
<xml_diff>
--- a/Info/balancing/metal system.xlsx
+++ b/Info/balancing/metal system.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Density</t>
   </si>
@@ -70,6 +70,24 @@
   </si>
   <si>
     <t>Health Entities</t>
+  </si>
+  <si>
+    <t>Chromium</t>
+  </si>
+  <si>
+    <t>Tin</t>
+  </si>
+  <si>
+    <t>Silver</t>
+  </si>
+  <si>
+    <t>Gold</t>
+  </si>
+  <si>
+    <t>Lead</t>
+  </si>
+  <si>
+    <t>Pipe Capacity</t>
   </si>
 </sst>
 </file>
@@ -199,13 +217,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="3" applyAlignment="1">
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="2" xfId="3" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="2" xfId="3" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="2" xfId="3" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -495,7 +513,7 @@
   <dimension ref="A1:T31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+      <selection activeCell="T2" sqref="T2:T31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -508,7 +526,9 @@
     <col min="6" max="6" width="23" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="12" width="9.140625" style="4"/>
+    <col min="9" max="10" width="9.140625" style="4"/>
+    <col min="11" max="11" width="14.140625" style="4" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="4"/>
     <col min="13" max="13" width="14" style="4" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14" style="4" customWidth="1"/>
     <col min="15" max="15" width="9.140625" style="4"/>
@@ -545,18 +565,22 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="J1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="6"/>
-      <c r="P1" s="6" t="s">
+      <c r="K1" s="7"/>
+      <c r="M1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="6"/>
-      <c r="S1" s="6" t="s">
+      <c r="N1" s="7"/>
+      <c r="P1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="6"/>
+      <c r="Q1" s="7"/>
+      <c r="S1" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="T1" s="7"/>
     </row>
     <row r="2" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -566,10 +590,10 @@
         <v>7.8739999999999997</v>
       </c>
       <c r="C2" s="3">
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="D2" s="3">
-        <v>13.4</v>
+        <v>28.5</v>
       </c>
       <c r="E2" s="3">
         <v>130</v>
@@ -583,29 +607,37 @@
       <c r="H2" s="3">
         <v>2862</v>
       </c>
-      <c r="M2" s="2" t="str">
+      <c r="J2" s="2" t="str">
         <f>A2</f>
         <v>Iron</v>
       </c>
+      <c r="K2" s="6">
+        <f>(F2-E2)/B2</f>
+        <v>8.89001778003556</v>
+      </c>
+      <c r="M2" s="2" t="str">
+        <f>J2</f>
+        <v>Iron</v>
+      </c>
       <c r="N2" s="5">
-        <f>(F2/(C2+B2))</f>
-        <v>16.162922256343947</v>
+        <f>F2/D2</f>
+        <v>7.0175438596491224</v>
       </c>
       <c r="P2" s="2" t="str">
         <f>M2</f>
         <v>Iron</v>
       </c>
-      <c r="Q2" s="7">
-        <f>((F2+E2)/D2)-C2</f>
-        <v>20.126865671641792</v>
+      <c r="Q2" s="5">
+        <f>(B2*C2)+E2</f>
+        <v>161.49600000000001</v>
       </c>
       <c r="S2" s="2" t="str">
         <f>P2</f>
         <v>Iron</v>
       </c>
-      <c r="T2" s="7">
-        <f>(((B2*C2)-D2)+F2)</f>
-        <v>222.03300000000002</v>
+      <c r="T2" s="5">
+        <f>(B2*C2)*D2</f>
+        <v>897.63599999999997</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -616,10 +648,10 @@
         <v>8.94</v>
       </c>
       <c r="C3" s="3">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="D3" s="3">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E3" s="3">
         <v>70</v>
@@ -633,29 +665,37 @@
       <c r="H3" s="3">
         <v>2562</v>
       </c>
+      <c r="J3" s="2" t="str">
+        <f>A3</f>
+        <v>Copper</v>
+      </c>
+      <c r="K3" s="6">
+        <f>(F3-E3)/B3</f>
+        <v>16.778523489932887</v>
+      </c>
       <c r="M3" s="2" t="str">
-        <f t="shared" ref="M3:M7" si="0">A3</f>
+        <f t="shared" ref="M3:M31" si="0">J3</f>
         <v>Copper</v>
       </c>
       <c r="N3" s="5">
-        <f t="shared" ref="N3:N7" si="1">(F3/(C3+B3))</f>
-        <v>18.819503849443969</v>
+        <f>F3/D3</f>
+        <v>12.941176470588236</v>
       </c>
       <c r="P3" s="2" t="str">
-        <f t="shared" ref="P3:P7" si="2">M3</f>
+        <f t="shared" ref="P3:P31" si="1">M3</f>
         <v>Copper</v>
       </c>
-      <c r="Q3" s="7">
-        <f t="shared" ref="Q3:Q7" si="3">((F3+E3)/D3)-C3</f>
-        <v>15.375</v>
+      <c r="Q3" s="5">
+        <f>(B3*C3)+E3</f>
+        <v>96.82</v>
       </c>
       <c r="S3" s="2" t="str">
-        <f t="shared" ref="S3:S7" si="4">P3</f>
+        <f t="shared" ref="S3:S31" si="2">P3</f>
         <v>Copper</v>
       </c>
-      <c r="T3" s="7">
-        <f t="shared" ref="T3:T7" si="5">(((B3*C3)-D3)+F3)</f>
-        <v>228.58500000000001</v>
+      <c r="T3" s="5">
+        <f t="shared" ref="T3:T31" si="3">(B3*C3)*D3</f>
+        <v>455.94</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
@@ -666,10 +706,10 @@
         <v>7.8</v>
       </c>
       <c r="C4" s="3">
-        <v>5</v>
+        <v>4.25</v>
       </c>
       <c r="D4" s="3">
-        <v>29.5</v>
+        <v>20</v>
       </c>
       <c r="E4" s="3">
         <v>250</v>
@@ -683,29 +723,37 @@
       <c r="H4" s="3">
         <v>2862</v>
       </c>
+      <c r="J4" s="2" t="str">
+        <f>A4</f>
+        <v>Steel</v>
+      </c>
+      <c r="K4" s="6">
+        <f>(F4-E4)/B4</f>
+        <v>19.23076923076923</v>
+      </c>
       <c r="M4" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Steel</v>
       </c>
       <c r="N4" s="5">
-        <f t="shared" si="1"/>
-        <v>31.25</v>
+        <f>F4/D4</f>
+        <v>20</v>
       </c>
       <c r="P4" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>Steel</v>
       </c>
-      <c r="Q4" s="7">
-        <f t="shared" si="3"/>
-        <v>17.033898305084747</v>
+      <c r="Q4" s="5">
+        <f>(B4*C4)+E4</f>
+        <v>283.14999999999998</v>
       </c>
       <c r="S4" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>Steel</v>
       </c>
-      <c r="T4" s="7">
-        <f t="shared" si="5"/>
-        <v>409.5</v>
+      <c r="T4" s="5">
+        <f t="shared" si="3"/>
+        <v>663</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
@@ -716,10 +764,10 @@
         <v>8.19</v>
       </c>
       <c r="C5" s="3">
-        <v>8.5</v>
+        <v>7.75</v>
       </c>
       <c r="D5" s="3">
-        <v>29.2</v>
+        <v>18</v>
       </c>
       <c r="E5" s="3">
         <v>520</v>
@@ -733,29 +781,37 @@
       <c r="H5" s="3">
         <v>2862</v>
       </c>
+      <c r="J5" s="2" t="str">
+        <f>A5</f>
+        <v>Stainless Steel</v>
+      </c>
+      <c r="K5" s="6">
+        <f>(F5-E5)/B5</f>
+        <v>41.514041514041516</v>
+      </c>
       <c r="M5" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Stainless Steel</v>
       </c>
       <c r="N5" s="5">
-        <f t="shared" si="1"/>
-        <v>51.527860994607558</v>
+        <f>F5/D5</f>
+        <v>47.777777777777779</v>
       </c>
       <c r="P5" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>Stainless Steel</v>
       </c>
-      <c r="Q5" s="7">
-        <f t="shared" si="3"/>
-        <v>38.760273972602739</v>
+      <c r="Q5" s="5">
+        <f>(B5*C5)+E5</f>
+        <v>583.47249999999997</v>
       </c>
       <c r="S5" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>Stainless Steel</v>
       </c>
-      <c r="T5" s="7">
-        <f t="shared" si="5"/>
-        <v>900.41499999999996</v>
+      <c r="T5" s="5">
+        <f t="shared" si="3"/>
+        <v>1142.5049999999999</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
@@ -772,36 +828,44 @@
         <v>11</v>
       </c>
       <c r="E6" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" s="3">
         <v>40</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
+      <c r="J6" s="2" t="str">
+        <f>A6</f>
+        <v>Wood</v>
+      </c>
+      <c r="K6" s="6">
+        <f>(F6-E6)/B6</f>
+        <v>5.2</v>
+      </c>
       <c r="M6" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Wood</v>
       </c>
       <c r="N6" s="5">
-        <f t="shared" si="1"/>
-        <v>4.1025641025641022</v>
+        <f>F6/D6</f>
+        <v>3.6363636363636362</v>
       </c>
       <c r="P6" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>Wood</v>
       </c>
-      <c r="Q6" s="7">
-        <f t="shared" si="3"/>
-        <v>1.3863636363636362</v>
+      <c r="Q6" s="5">
+        <f>(B6*C6)+E6</f>
+        <v>17.875</v>
       </c>
       <c r="S6" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>Wood</v>
       </c>
-      <c r="T6" s="7">
-        <f t="shared" si="5"/>
-        <v>45.875</v>
+      <c r="T6" s="5">
+        <f t="shared" si="3"/>
+        <v>185.625</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
@@ -809,7 +873,7 @@
         <v>13</v>
       </c>
       <c r="B7" s="3">
-        <v>2.5499999999999998</v>
+        <v>12.55</v>
       </c>
       <c r="C7" s="3">
         <v>5</v>
@@ -818,7 +882,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" s="3">
         <v>15</v>
@@ -829,80 +893,328 @@
       <c r="H7" s="3">
         <v>5000</v>
       </c>
+      <c r="J7" s="2" t="str">
+        <f>A7</f>
+        <v>Stone</v>
+      </c>
+      <c r="K7" s="6">
+        <f>(F7-E7)/B7</f>
+        <v>1.1155378486055776</v>
+      </c>
       <c r="M7" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Stone</v>
       </c>
       <c r="N7" s="5">
-        <f t="shared" si="1"/>
-        <v>1.9867549668874174</v>
+        <f>F7/D7</f>
+        <v>15</v>
       </c>
       <c r="P7" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>Stone</v>
       </c>
-      <c r="Q7" s="7">
-        <f t="shared" si="3"/>
-        <v>10</v>
+      <c r="Q7" s="5">
+        <f>(B7*C7)+E7</f>
+        <v>63.75</v>
       </c>
       <c r="S7" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>Stone</v>
       </c>
-      <c r="T7" s="7">
-        <f t="shared" si="5"/>
-        <v>26.75</v>
+      <c r="T7" s="5">
+        <f t="shared" si="3"/>
+        <v>62.75</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
+      <c r="A8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="3">
+        <v>7.19</v>
+      </c>
+      <c r="C8" s="3">
+        <v>8.5</v>
+      </c>
+      <c r="D8" s="3">
+        <v>36</v>
+      </c>
+      <c r="E8" s="3">
+        <v>160</v>
+      </c>
+      <c r="F8" s="3">
+        <v>280</v>
+      </c>
+      <c r="G8" s="3">
+        <v>1860</v>
+      </c>
+      <c r="H8" s="3">
+        <v>2670</v>
+      </c>
+      <c r="J8" s="2" t="str">
+        <f>A8</f>
+        <v>Chromium</v>
+      </c>
+      <c r="K8" s="6">
+        <f>(F8-E8)/B8</f>
+        <v>16.689847009735743</v>
+      </c>
+      <c r="M8" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Chromium</v>
+      </c>
+      <c r="N8" s="5">
+        <f>F8/D8</f>
+        <v>7.7777777777777777</v>
+      </c>
+      <c r="P8" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Chromium</v>
+      </c>
+      <c r="Q8" s="5">
+        <f>(B8*C8)+E8</f>
+        <v>221.11500000000001</v>
+      </c>
+      <c r="S8" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Chromium</v>
+      </c>
+      <c r="T8" s="5">
+        <f t="shared" si="3"/>
+        <v>2200.14</v>
+      </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
+      <c r="A9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="3">
+        <v>7.28</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="D9" s="3">
+        <v>47</v>
+      </c>
+      <c r="E9" s="3">
+        <v>9</v>
+      </c>
+      <c r="F9" s="3">
+        <v>19</v>
+      </c>
+      <c r="G9" s="3">
+        <v>232</v>
+      </c>
+      <c r="H9" s="3">
+        <v>2600</v>
+      </c>
+      <c r="J9" s="2" t="str">
+        <f>A9</f>
+        <v>Tin</v>
+      </c>
+      <c r="K9" s="6">
+        <f>(F9-E9)/B9</f>
+        <v>1.3736263736263736</v>
+      </c>
+      <c r="M9" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Tin</v>
+      </c>
+      <c r="N9" s="5">
+        <f>F9/D9</f>
+        <v>0.40425531914893614</v>
+      </c>
+      <c r="P9" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Tin</v>
+      </c>
+      <c r="Q9" s="5">
+        <f>(B9*C9)+E9</f>
+        <v>19.920000000000002</v>
+      </c>
+      <c r="S9" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Tin</v>
+      </c>
+      <c r="T9" s="5">
+        <f t="shared" si="3"/>
+        <v>513.24</v>
+      </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
+      <c r="A10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="3">
+        <v>10.49</v>
+      </c>
+      <c r="C10" s="3">
+        <v>2.75</v>
+      </c>
+      <c r="D10" s="3">
+        <v>10.5</v>
+      </c>
+      <c r="E10" s="3">
+        <v>55</v>
+      </c>
+      <c r="F10" s="3">
+        <v>360</v>
+      </c>
+      <c r="G10" s="3">
+        <v>961</v>
+      </c>
+      <c r="H10" s="3">
+        <v>2212</v>
+      </c>
+      <c r="J10" s="2" t="str">
+        <f>A10</f>
+        <v>Silver</v>
+      </c>
+      <c r="K10" s="6">
+        <f>(F10-E10)/B10</f>
+        <v>29.07530981887512</v>
+      </c>
+      <c r="M10" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Silver</v>
+      </c>
+      <c r="N10" s="5">
+        <f>F10/D10</f>
+        <v>34.285714285714285</v>
+      </c>
+      <c r="P10" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Silver</v>
+      </c>
+      <c r="Q10" s="5">
+        <f>(B10*C10)+E10</f>
+        <v>83.847499999999997</v>
+      </c>
+      <c r="S10" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Silver</v>
+      </c>
+      <c r="T10" s="5">
+        <f t="shared" si="3"/>
+        <v>302.89875000000001</v>
+      </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
+      <c r="A11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="3">
+        <v>19.32</v>
+      </c>
+      <c r="C11" s="3">
+        <v>2.75</v>
+      </c>
+      <c r="D11" s="3">
+        <v>10.8</v>
+      </c>
+      <c r="E11" s="3">
+        <v>190</v>
+      </c>
+      <c r="F11" s="3">
+        <v>220</v>
+      </c>
+      <c r="G11" s="3">
+        <v>1063</v>
+      </c>
+      <c r="H11" s="3">
+        <v>2800</v>
+      </c>
+      <c r="J11" s="2" t="str">
+        <f>A11</f>
+        <v>Gold</v>
+      </c>
+      <c r="K11" s="6">
+        <f>(F11-E11)/B11</f>
+        <v>1.5527950310559007</v>
+      </c>
+      <c r="M11" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Gold</v>
+      </c>
+      <c r="N11" s="5">
+        <f>F11/D11</f>
+        <v>20.37037037037037</v>
+      </c>
+      <c r="P11" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Gold</v>
+      </c>
+      <c r="Q11" s="5">
+        <f>(B11*C11)+E11</f>
+        <v>243.13</v>
+      </c>
+      <c r="S11" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Gold</v>
+      </c>
+      <c r="T11" s="5">
+        <f t="shared" si="3"/>
+        <v>573.80400000000009</v>
+      </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
+      <c r="A12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="3">
+        <v>11.34</v>
+      </c>
+      <c r="C12" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="D12" s="3">
+        <v>2</v>
+      </c>
+      <c r="E12" s="3">
+        <v>19</v>
+      </c>
+      <c r="F12" s="3">
+        <v>32</v>
+      </c>
+      <c r="G12" s="3">
+        <v>327</v>
+      </c>
+      <c r="H12" s="3">
+        <v>1750</v>
+      </c>
+      <c r="J12" s="2" t="str">
+        <f>A12</f>
+        <v>Lead</v>
+      </c>
+      <c r="K12" s="6">
+        <f>(F12-E12)/B12</f>
+        <v>1.1463844797178131</v>
+      </c>
+      <c r="M12" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Lead</v>
+      </c>
+      <c r="N12" s="5">
+        <f>F12/D12</f>
+        <v>16</v>
+      </c>
+      <c r="P12" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Lead</v>
+      </c>
+      <c r="Q12" s="5">
+        <f>(B12*C12)+E12</f>
+        <v>36.01</v>
+      </c>
+      <c r="S12" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Lead</v>
+      </c>
+      <c r="T12" s="5">
+        <f t="shared" si="3"/>
+        <v>34.019999999999996</v>
+      </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
@@ -913,6 +1225,38 @@
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
+      <c r="J13" s="2">
+        <f>A13</f>
+        <v>0</v>
+      </c>
+      <c r="K13" s="6" t="e">
+        <f>(F13-E13)/B13</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M13" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N13" s="5" t="e">
+        <f>F13/D13</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P13" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q13" s="5">
+        <f>(B13*C13)+E13</f>
+        <v>0</v>
+      </c>
+      <c r="S13" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T13" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
@@ -923,6 +1267,38 @@
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
+      <c r="J14" s="2">
+        <f>A14</f>
+        <v>0</v>
+      </c>
+      <c r="K14" s="6" t="e">
+        <f>(F14-E14)/B14</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M14" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N14" s="5" t="e">
+        <f>F14/D14</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P14" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q14" s="5">
+        <f>(B14*C14)+E14</f>
+        <v>0</v>
+      </c>
+      <c r="S14" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T14" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
@@ -933,6 +1309,38 @@
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
+      <c r="J15" s="2">
+        <f>A15</f>
+        <v>0</v>
+      </c>
+      <c r="K15" s="6" t="e">
+        <f>(F15-E15)/B15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M15" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N15" s="5" t="e">
+        <f>F15/D15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P15" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q15" s="5">
+        <f>(B15*C15)+E15</f>
+        <v>0</v>
+      </c>
+      <c r="S15" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T15" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
@@ -943,8 +1351,40 @@
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J16" s="2">
+        <f>A16</f>
+        <v>0</v>
+      </c>
+      <c r="K16" s="6" t="e">
+        <f>(F16-E16)/B16</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M16" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N16" s="5" t="e">
+        <f>F16/D16</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P16" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q16" s="5">
+        <f>(B16*C16)+E16</f>
+        <v>0</v>
+      </c>
+      <c r="S16" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T16" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -953,8 +1393,40 @@
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J17" s="2">
+        <f>A17</f>
+        <v>0</v>
+      </c>
+      <c r="K17" s="6" t="e">
+        <f>(F17-E17)/B17</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M17" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N17" s="5" t="e">
+        <f>F17/D17</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P17" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q17" s="5">
+        <f>(B17*C17)+E17</f>
+        <v>0</v>
+      </c>
+      <c r="S17" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T17" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -963,8 +1435,40 @@
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J18" s="2">
+        <f>A18</f>
+        <v>0</v>
+      </c>
+      <c r="K18" s="6" t="e">
+        <f>(F18-E18)/B18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M18" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N18" s="5" t="e">
+        <f>F18/D18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P18" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q18" s="5">
+        <f>(B18*C18)+E18</f>
+        <v>0</v>
+      </c>
+      <c r="S18" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T18" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -973,8 +1477,40 @@
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J19" s="2">
+        <f>A19</f>
+        <v>0</v>
+      </c>
+      <c r="K19" s="6" t="e">
+        <f>(F19-E19)/B19</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M19" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N19" s="5" t="e">
+        <f>F19/D19</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P19" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q19" s="5">
+        <f>(B19*C19)+E19</f>
+        <v>0</v>
+      </c>
+      <c r="S19" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T19" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -983,8 +1519,40 @@
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J20" s="2">
+        <f>A20</f>
+        <v>0</v>
+      </c>
+      <c r="K20" s="6" t="e">
+        <f>(F20-E20)/B20</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M20" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N20" s="5" t="e">
+        <f>F20/D20</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P20" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q20" s="5">
+        <f>(B20*C20)+E20</f>
+        <v>0</v>
+      </c>
+      <c r="S20" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T20" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -993,8 +1561,40 @@
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J21" s="2">
+        <f>A21</f>
+        <v>0</v>
+      </c>
+      <c r="K21" s="6" t="e">
+        <f>(F21-E21)/B21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M21" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N21" s="5" t="e">
+        <f>F21/D21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P21" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q21" s="5">
+        <f>(B21*C21)+E21</f>
+        <v>0</v>
+      </c>
+      <c r="S21" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T21" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -1003,8 +1603,40 @@
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J22" s="2">
+        <f>A22</f>
+        <v>0</v>
+      </c>
+      <c r="K22" s="6" t="e">
+        <f>(F22-E22)/B22</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M22" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N22" s="5" t="e">
+        <f>F22/D22</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P22" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q22" s="5">
+        <f>(B22*C22)+E22</f>
+        <v>0</v>
+      </c>
+      <c r="S22" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T22" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -1013,8 +1645,40 @@
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J23" s="2">
+        <f>A23</f>
+        <v>0</v>
+      </c>
+      <c r="K23" s="6" t="e">
+        <f>(F23-E23)/B23</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M23" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N23" s="5" t="e">
+        <f>F23/D23</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P23" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q23" s="5">
+        <f>(B23*C23)+E23</f>
+        <v>0</v>
+      </c>
+      <c r="S23" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T23" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1023,8 +1687,40 @@
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J24" s="2">
+        <f>A24</f>
+        <v>0</v>
+      </c>
+      <c r="K24" s="6" t="e">
+        <f>(F24-E24)/B24</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M24" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N24" s="5" t="e">
+        <f>F24/D24</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P24" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q24" s="5">
+        <f>(B24*C24)+E24</f>
+        <v>0</v>
+      </c>
+      <c r="S24" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T24" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1033,8 +1729,40 @@
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J25" s="2">
+        <f>A25</f>
+        <v>0</v>
+      </c>
+      <c r="K25" s="6" t="e">
+        <f>(F25-E25)/B25</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M25" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N25" s="5" t="e">
+        <f>F25/D25</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P25" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q25" s="5">
+        <f>(B25*C25)+E25</f>
+        <v>0</v>
+      </c>
+      <c r="S25" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T25" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1043,8 +1771,40 @@
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J26" s="2">
+        <f>A26</f>
+        <v>0</v>
+      </c>
+      <c r="K26" s="6" t="e">
+        <f>(F26-E26)/B26</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M26" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N26" s="5" t="e">
+        <f>F26/D26</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P26" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q26" s="5">
+        <f>(B26*C26)+E26</f>
+        <v>0</v>
+      </c>
+      <c r="S26" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T26" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -1053,8 +1813,40 @@
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J27" s="2">
+        <f>A27</f>
+        <v>0</v>
+      </c>
+      <c r="K27" s="6" t="e">
+        <f>(F27-E27)/B27</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M27" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N27" s="5" t="e">
+        <f>F27/D27</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P27" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q27" s="5">
+        <f>(B27*C27)+E27</f>
+        <v>0</v>
+      </c>
+      <c r="S27" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T27" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -1063,8 +1855,40 @@
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J28" s="2">
+        <f>A28</f>
+        <v>0</v>
+      </c>
+      <c r="K28" s="6" t="e">
+        <f>(F28-E28)/B28</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M28" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N28" s="5" t="e">
+        <f>F28/D28</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P28" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q28" s="5">
+        <f>(B28*C28)+E28</f>
+        <v>0</v>
+      </c>
+      <c r="S28" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T28" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -1073,8 +1897,40 @@
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J29" s="2">
+        <f>A29</f>
+        <v>0</v>
+      </c>
+      <c r="K29" s="6" t="e">
+        <f>(F29-E29)/B29</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M29" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N29" s="5" t="e">
+        <f>F29/D29</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P29" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q29" s="5">
+        <f>(B29*C29)+E29</f>
+        <v>0</v>
+      </c>
+      <c r="S29" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T29" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -1083,8 +1939,40 @@
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J30" s="2">
+        <f>A30</f>
+        <v>0</v>
+      </c>
+      <c r="K30" s="6" t="e">
+        <f>(F30-E30)/B30</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M30" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N30" s="5" t="e">
+        <f>F30/D30</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P30" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q30" s="5">
+        <f>(B30*C30)+E30</f>
+        <v>0</v>
+      </c>
+      <c r="S30" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T30" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -1093,11 +1981,44 @@
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
+      <c r="J31" s="2">
+        <f>A31</f>
+        <v>0</v>
+      </c>
+      <c r="K31" s="6" t="e">
+        <f>(F31-E31)/B31</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M31" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N31" s="5" t="e">
+        <f>F31/D31</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P31" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q31" s="5">
+        <f>(B31*C31)+E31</f>
+        <v>0</v>
+      </c>
+      <c r="S31" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T31" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="J1:K1"/>
     <mergeCell ref="S1:T1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Electric Mining Drills added to use Material System
</commit_message>
<xml_diff>
--- a/Info/balancing/metal system.xlsx
+++ b/Info/balancing/metal system.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Materials" sheetId="2" r:id="rId1"/>
     <sheet name="Part 1" sheetId="1" r:id="rId2"/>
+    <sheet name="Part 2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Density</t>
   </si>
@@ -131,6 +132,9 @@
   </si>
   <si>
     <t>Accumulator Storage</t>
+  </si>
+  <si>
+    <t>Mining Speed</t>
   </si>
 </sst>
 </file>
@@ -561,7 +565,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{028B0D2B-13D9-4234-8CF2-6AB8658F4FDF}">
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -1205,8 +1209,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H34" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1384,7 +1388,7 @@
         <v>14.92</v>
       </c>
       <c r="M3" s="5">
-        <f t="shared" ref="M3:N31" si="0">L3*5</f>
+        <f t="shared" ref="M3:M31" si="0">L3*5</f>
         <v>74.599999999999994</v>
       </c>
       <c r="N3" s="5">
@@ -3020,4 +3024,720 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA1EAC7A-C1C3-430F-84F9-F38621A782F4}">
+  <dimension ref="A1:N31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="15.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.140625" style="4"/>
+    <col min="16" max="16" width="15.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.28515625" style="4" customWidth="1"/>
+    <col min="18" max="18" width="15.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.28515625" style="4" customWidth="1"/>
+    <col min="20" max="20" width="15.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.7109375" style="4" customWidth="1"/>
+    <col min="22" max="22" width="15.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+    </row>
+    <row r="2" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="str">
+        <f>Materials!A2</f>
+        <v>Iron</v>
+      </c>
+      <c r="B2" s="6">
+        <f>Materials!D2/2</f>
+        <v>14.25</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="str">
+        <f>Materials!A3</f>
+        <v>Copper</v>
+      </c>
+      <c r="B3" s="6">
+        <f>Materials!D3/2</f>
+        <v>8.5</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="str">
+        <f>Materials!A4</f>
+        <v>Steel</v>
+      </c>
+      <c r="B4" s="6">
+        <f>Materials!D4/2</f>
+        <v>10</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="str">
+        <f>Materials!A5</f>
+        <v>Wood</v>
+      </c>
+      <c r="B5" s="6">
+        <f>Materials!D5/2</f>
+        <v>5.5</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="str">
+        <f>Materials!A6</f>
+        <v>Stone</v>
+      </c>
+      <c r="B6" s="6">
+        <f>Materials!D6/2</f>
+        <v>0.5</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="str">
+        <f>Materials!A7</f>
+        <v>Chromium</v>
+      </c>
+      <c r="B7" s="6">
+        <f>Materials!D7/2</f>
+        <v>18</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="str">
+        <f>Materials!A8</f>
+        <v>Tin</v>
+      </c>
+      <c r="B8" s="6">
+        <f>Materials!D8/2</f>
+        <v>23.5</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="str">
+        <f>Materials!A9</f>
+        <v>Silver</v>
+      </c>
+      <c r="B9" s="6">
+        <f>Materials!D9/2</f>
+        <v>5.25</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="str">
+        <f>Materials!A10</f>
+        <v>Gold</v>
+      </c>
+      <c r="B10" s="6">
+        <f>Materials!D10/2</f>
+        <v>5.4</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="str">
+        <f>Materials!A11</f>
+        <v>Lead</v>
+      </c>
+      <c r="B11" s="6">
+        <f>Materials!D11/2</f>
+        <v>1</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="str">
+        <f>Materials!A12</f>
+        <v>Obsidian</v>
+      </c>
+      <c r="B12" s="6">
+        <f>Materials!D12/2</f>
+        <v>6.75</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="str">
+        <f>Materials!A13</f>
+        <v>Rubber</v>
+      </c>
+      <c r="B13" s="6">
+        <f>Materials!D13/2</f>
+        <v>50</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <f>Materials!A14</f>
+        <v>0</v>
+      </c>
+      <c r="B14" s="6">
+        <f>Materials!D14/2</f>
+        <v>0</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="str">
+        <f>Materials!A15</f>
+        <v>Stainless Steel</v>
+      </c>
+      <c r="B15" s="6">
+        <f>Materials!D15/2</f>
+        <v>28</v>
+      </c>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="str">
+        <f>Materials!A16</f>
+        <v>Bronze</v>
+      </c>
+      <c r="B16" s="6">
+        <f>Materials!D16/2</f>
+        <v>32</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <f>Materials!A17</f>
+        <v>0</v>
+      </c>
+      <c r="B17" s="6">
+        <f>Materials!D17/2</f>
+        <v>0</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <f>Materials!A18</f>
+        <v>0</v>
+      </c>
+      <c r="B18" s="6">
+        <f>Materials!D18/2</f>
+        <v>0</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <f>Materials!A19</f>
+        <v>0</v>
+      </c>
+      <c r="B19" s="6">
+        <f>Materials!D19/2</f>
+        <v>0</v>
+      </c>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <f>Materials!A20</f>
+        <v>0</v>
+      </c>
+      <c r="B20" s="6">
+        <f>Materials!D20/2</f>
+        <v>0</v>
+      </c>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <f>Materials!A21</f>
+        <v>0</v>
+      </c>
+      <c r="B21" s="6">
+        <f>Materials!D21/2</f>
+        <v>0</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <f>Materials!A22</f>
+        <v>0</v>
+      </c>
+      <c r="B22" s="6">
+        <f>Materials!D22/2</f>
+        <v>0</v>
+      </c>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <f>Materials!A23</f>
+        <v>0</v>
+      </c>
+      <c r="B23" s="6">
+        <f>Materials!D23/2</f>
+        <v>0</v>
+      </c>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <f>Materials!A24</f>
+        <v>0</v>
+      </c>
+      <c r="B24" s="6">
+        <f>Materials!D24/2</f>
+        <v>0</v>
+      </c>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <f>Materials!A25</f>
+        <v>0</v>
+      </c>
+      <c r="B25" s="6">
+        <f>Materials!D25/2</f>
+        <v>0</v>
+      </c>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <f>Materials!A26</f>
+        <v>0</v>
+      </c>
+      <c r="B26" s="6">
+        <f>Materials!D26/2</f>
+        <v>0</v>
+      </c>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+      <c r="N26" s="5"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <f>Materials!A27</f>
+        <v>0</v>
+      </c>
+      <c r="B27" s="6">
+        <f>Materials!D27/2</f>
+        <v>0</v>
+      </c>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <f>Materials!A28</f>
+        <v>0</v>
+      </c>
+      <c r="B28" s="6">
+        <f>Materials!D28/2</f>
+        <v>0</v>
+      </c>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="5"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <f>Materials!A29</f>
+        <v>0</v>
+      </c>
+      <c r="B29" s="6">
+        <f>Materials!D29/2</f>
+        <v>0</v>
+      </c>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="5"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <f>Materials!A30</f>
+        <v>0</v>
+      </c>
+      <c r="B30" s="6">
+        <f>Materials!D30/2</f>
+        <v>0</v>
+      </c>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
+      <c r="N30" s="5"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <f>Materials!A31</f>
+        <v>0</v>
+      </c>
+      <c r="B31" s="6">
+        <f>Materials!D31/2</f>
+        <v>0</v>
+      </c>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Cadmium and Tungsten Ore
</commit_message>
<xml_diff>
--- a/Info/balancing/metal system.xlsx
+++ b/Info/balancing/metal system.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Density</t>
   </si>
@@ -135,12 +135,21 @@
   </si>
   <si>
     <t>Mining Speed</t>
+  </si>
+  <si>
+    <t>Cadmium</t>
+  </si>
+  <si>
+    <t>Tungsten</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -250,7 +259,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -277,6 +286,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -566,7 +578,7 @@
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -951,100 +963,136 @@
       <c r="I13" s="3"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
+      <c r="A14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="3">
+        <v>8.65</v>
+      </c>
+      <c r="C14" s="3">
+        <v>2</v>
+      </c>
+      <c r="D14" s="3">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E14" s="3">
+        <v>1.46</v>
+      </c>
+      <c r="F14" s="3">
+        <v>25</v>
+      </c>
+      <c r="G14" s="3">
+        <v>78</v>
+      </c>
+      <c r="H14" s="3">
+        <v>321</v>
+      </c>
+      <c r="I14" s="3">
+        <v>767</v>
+      </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="B15" s="9">
-        <f>B4+B7</f>
-        <v>14.99</v>
+        <v>19.25</v>
       </c>
       <c r="C15" s="9">
-        <f t="shared" ref="C15:G15" si="0">C4+C7</f>
-        <v>12.75</v>
-      </c>
-      <c r="D15" s="8">
-        <f t="shared" si="0"/>
-        <v>56</v>
+        <v>7.5</v>
+      </c>
+      <c r="D15" s="10">
+        <v>40.5</v>
       </c>
       <c r="E15" s="9">
-        <f t="shared" si="0"/>
-        <v>11.309999999999999</v>
+        <v>1.82</v>
       </c>
       <c r="F15" s="8">
-        <f t="shared" si="0"/>
-        <v>410</v>
+        <v>500</v>
       </c>
       <c r="G15" s="8">
-        <f t="shared" si="0"/>
-        <v>680</v>
+        <v>1000</v>
       </c>
       <c r="H15" s="8">
-        <f>AVERAGE(H4,H7)</f>
-        <v>1642.5</v>
+        <v>3422</v>
       </c>
       <c r="I15" s="8">
-        <f>AVERAGE(I4,I7)</f>
-        <v>2766</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="9">
+        <f>B5+B8</f>
+        <v>14.780000000000001</v>
+      </c>
+      <c r="C16" s="9">
+        <f t="shared" ref="C16:I16" si="0">C5+C8</f>
+        <v>3.75</v>
+      </c>
+      <c r="D16" s="8">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="E16" s="9">
+        <f t="shared" si="0"/>
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="F16" s="8">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G16" s="8">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="H16" s="8">
+        <f>AVERAGE(H5,H8)</f>
+        <v>232</v>
+      </c>
+      <c r="I16" s="8">
+        <f>AVERAGE(I5,I8)</f>
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="9">
-        <f>B3+B8</f>
-        <v>16.22</v>
-      </c>
-      <c r="C16" s="9">
-        <f t="shared" ref="C16:G16" si="1">C3+C8</f>
-        <v>4.5</v>
-      </c>
-      <c r="D16" s="8">
+      <c r="B17" s="9">
+        <f>B4+B9</f>
+        <v>18.29</v>
+      </c>
+      <c r="C17" s="9">
+        <f t="shared" ref="C17:I17" si="1">C4+C9</f>
+        <v>7</v>
+      </c>
+      <c r="D17" s="8">
         <f t="shared" si="1"/>
-        <v>64</v>
-      </c>
-      <c r="E16" s="9">
+        <v>30.5</v>
+      </c>
+      <c r="E17" s="9">
         <f t="shared" si="1"/>
-        <v>14.68</v>
-      </c>
-      <c r="F16" s="8">
+        <v>12.51</v>
+      </c>
+      <c r="F17" s="8">
         <f t="shared" si="1"/>
-        <v>79</v>
-      </c>
-      <c r="G16" s="8">
+        <v>305</v>
+      </c>
+      <c r="G17" s="8">
         <f t="shared" si="1"/>
-        <v>239</v>
-      </c>
-      <c r="H16" s="8">
-        <f>AVERAGE(H3,H8)</f>
-        <v>658</v>
-      </c>
-      <c r="I16" s="8">
-        <f>AVERAGE(I3,I8)</f>
-        <v>2581</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
+        <v>760</v>
+      </c>
+      <c r="H17" s="8">
+        <f>AVERAGE(H4,H9)</f>
+        <v>1193</v>
+      </c>
+      <c r="I17" s="8">
+        <f>AVERAGE(I4,I9)</f>
+        <v>2537</v>
+      </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
@@ -1209,8 +1257,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H34" sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1977,235 +2025,235 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
+      <c r="A14" s="2" t="str">
         <f>Materials!A14</f>
-        <v>0</v>
+        <v>Cadmium</v>
       </c>
       <c r="B14" s="6">
         <f>((Materials!D14/2)+Materials!B14)</f>
-        <v>0</v>
-      </c>
-      <c r="C14" s="5" t="e">
+        <v>10.95</v>
+      </c>
+      <c r="C14" s="5">
         <f>(Materials!G14/Materials!D14)+2</f>
-        <v>#DIV/0!</v>
+        <v>18.956521739130437</v>
       </c>
       <c r="D14" s="5">
         <f>(Materials!B14*Materials!C14)+Materials!F14</f>
-        <v>0</v>
+        <v>42.3</v>
       </c>
       <c r="E14" s="5">
         <f>(Materials!B14*Materials!C14)*Materials!D14</f>
-        <v>0</v>
+        <v>79.58</v>
       </c>
       <c r="F14" s="5">
         <f>((Materials!B14*Materials!C14)/2)+5</f>
-        <v>5</v>
-      </c>
-      <c r="G14" s="6" t="e">
+        <v>13.65</v>
+      </c>
+      <c r="G14" s="6">
         <f>Materials!D14/Materials!C14</f>
-        <v>#DIV/0!</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="H14" s="5">
         <f>60+Materials!D14</f>
-        <v>60</v>
-      </c>
-      <c r="I14" s="6" t="e">
+        <v>64.599999999999994</v>
+      </c>
+      <c r="I14" s="6">
         <f>Materials!G14/Materials!D14</f>
-        <v>#DIV/0!</v>
+        <v>16.956521739130437</v>
       </c>
       <c r="J14" s="5">
         <f>Materials!G14*Materials!E14</f>
-        <v>0</v>
+        <v>113.88</v>
       </c>
       <c r="K14" s="5">
         <f>Materials!E14+Materials!C14</f>
-        <v>0</v>
+        <v>3.46</v>
       </c>
       <c r="L14" s="5">
         <f>Materials!E14+Materials!B14</f>
-        <v>0</v>
+        <v>10.11</v>
       </c>
       <c r="M14" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>50.55</v>
       </c>
       <c r="N14" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1138.8</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="str">
         <f>Materials!A15</f>
-        <v>Stainless Steel</v>
+        <v>Tungsten</v>
       </c>
       <c r="B15" s="6">
         <f>((Materials!D15/2)+Materials!B15)</f>
-        <v>42.99</v>
+        <v>39.5</v>
       </c>
       <c r="C15" s="5">
         <f>(Materials!G15/Materials!D15)+2</f>
-        <v>14.142857142857142</v>
+        <v>26.691358024691358</v>
       </c>
       <c r="D15" s="5">
         <f>(Materials!B15*Materials!C15)+Materials!F15</f>
-        <v>601.12249999999995</v>
+        <v>644.375</v>
       </c>
       <c r="E15" s="5">
         <f>(Materials!B15*Materials!C15)*Materials!D15</f>
-        <v>10702.86</v>
+        <v>5847.1875</v>
       </c>
       <c r="F15" s="5">
         <f>((Materials!B15*Materials!C15)/2)+5</f>
-        <v>100.56125</v>
+        <v>77.1875</v>
       </c>
       <c r="G15" s="6">
         <f>Materials!D15/Materials!C15</f>
-        <v>4.3921568627450984</v>
+        <v>5.4</v>
       </c>
       <c r="H15" s="5">
         <f>60+Materials!D15</f>
-        <v>116</v>
+        <v>100.5</v>
       </c>
       <c r="I15" s="6">
         <f>Materials!G15/Materials!D15</f>
-        <v>12.142857142857142</v>
+        <v>24.691358024691358</v>
       </c>
       <c r="J15" s="5">
         <f>Materials!G15*Materials!E15</f>
-        <v>7690.7999999999993</v>
+        <v>1820</v>
       </c>
       <c r="K15" s="5">
         <f>Materials!E15+Materials!C15</f>
-        <v>24.06</v>
+        <v>9.32</v>
       </c>
       <c r="L15" s="5">
         <f>Materials!E15+Materials!B15</f>
-        <v>26.299999999999997</v>
+        <v>21.07</v>
       </c>
       <c r="M15" s="5">
         <f t="shared" si="0"/>
-        <v>131.5</v>
+        <v>105.35</v>
       </c>
       <c r="N15" s="5">
         <f t="shared" si="1"/>
-        <v>76908</v>
+        <v>18200</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="str">
         <f>Materials!A16</f>
-        <v>Bronze</v>
+        <v>Stainless Steel</v>
       </c>
       <c r="B16" s="6">
         <f>((Materials!D16/2)+Materials!B16)</f>
-        <v>48.22</v>
+        <v>43.78</v>
       </c>
       <c r="C16" s="5">
         <f>(Materials!G16/Materials!D16)+2</f>
-        <v>5.734375</v>
+        <v>3.0172413793103448</v>
       </c>
       <c r="D16" s="5">
         <f>(Materials!B16*Materials!C16)+Materials!F16</f>
-        <v>151.99</v>
+        <v>65.425000000000011</v>
       </c>
       <c r="E16" s="5">
         <f>(Materials!B16*Materials!C16)*Materials!D16</f>
-        <v>4671.3599999999997</v>
+        <v>3214.65</v>
       </c>
       <c r="F16" s="5">
         <f>((Materials!B16*Materials!C16)/2)+5</f>
-        <v>41.494999999999997</v>
+        <v>32.712500000000006</v>
       </c>
       <c r="G16" s="6">
         <f>Materials!D16/Materials!C16</f>
-        <v>14.222222222222221</v>
+        <v>15.466666666666667</v>
       </c>
       <c r="H16" s="5">
         <f>60+Materials!D16</f>
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="I16" s="6">
         <f>Materials!G16/Materials!D16</f>
-        <v>3.734375</v>
+        <v>1.0172413793103448</v>
       </c>
       <c r="J16" s="5">
         <f>Materials!G16*Materials!E16</f>
-        <v>3508.52</v>
+        <v>513.29999999999995</v>
       </c>
       <c r="K16" s="5">
         <f>Materials!E16+Materials!C16</f>
-        <v>19.18</v>
+        <v>12.45</v>
       </c>
       <c r="L16" s="5">
         <f>Materials!E16+Materials!B16</f>
-        <v>30.9</v>
+        <v>23.48</v>
       </c>
       <c r="M16" s="5">
         <f t="shared" si="0"/>
-        <v>154.5</v>
+        <v>117.4</v>
       </c>
       <c r="N16" s="5">
         <f t="shared" si="1"/>
-        <v>35085.199999999997</v>
+        <v>5133</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
+      <c r="A17" s="2" t="str">
         <f>Materials!A17</f>
-        <v>0</v>
+        <v>Bronze</v>
       </c>
       <c r="B17" s="6">
         <f>((Materials!D17/2)+Materials!B17)</f>
-        <v>0</v>
-      </c>
-      <c r="C17" s="5" t="e">
+        <v>33.54</v>
+      </c>
+      <c r="C17" s="5">
         <f>(Materials!G17/Materials!D17)+2</f>
-        <v>#DIV/0!</v>
+        <v>26.918032786885245</v>
       </c>
       <c r="D17" s="5">
         <f>(Materials!B17*Materials!C17)+Materials!F17</f>
-        <v>0</v>
+        <v>433.03</v>
       </c>
       <c r="E17" s="5">
         <f>(Materials!B17*Materials!C17)*Materials!D17</f>
-        <v>0</v>
+        <v>3904.915</v>
       </c>
       <c r="F17" s="5">
         <f>((Materials!B17*Materials!C17)/2)+5</f>
-        <v>5</v>
-      </c>
-      <c r="G17" s="6" t="e">
+        <v>69.015000000000001</v>
+      </c>
+      <c r="G17" s="6">
         <f>Materials!D17/Materials!C17</f>
-        <v>#DIV/0!</v>
+        <v>4.3571428571428568</v>
       </c>
       <c r="H17" s="5">
         <f>60+Materials!D17</f>
-        <v>60</v>
-      </c>
-      <c r="I17" s="6" t="e">
+        <v>90.5</v>
+      </c>
+      <c r="I17" s="6">
         <f>Materials!G17/Materials!D17</f>
-        <v>#DIV/0!</v>
+        <v>24.918032786885245</v>
       </c>
       <c r="J17" s="5">
         <f>Materials!G17*Materials!E17</f>
-        <v>0</v>
+        <v>9507.6</v>
       </c>
       <c r="K17" s="5">
         <f>Materials!E17+Materials!C17</f>
-        <v>0</v>
+        <v>19.509999999999998</v>
       </c>
       <c r="L17" s="5">
         <f>Materials!E17+Materials!B17</f>
-        <v>0</v>
+        <v>30.799999999999997</v>
       </c>
       <c r="M17" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>154</v>
       </c>
       <c r="N17" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>95076</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
@@ -3031,7 +3079,7 @@
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3342,13 +3390,13 @@
       <c r="N13" s="5"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
+      <c r="A14" s="2" t="str">
         <f>Materials!A14</f>
-        <v>0</v>
+        <v>Cadmium</v>
       </c>
       <c r="B14" s="6">
         <f>Materials!D14/2</f>
-        <v>0</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -3366,11 +3414,11 @@
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="str">
         <f>Materials!A15</f>
-        <v>Stainless Steel</v>
+        <v>Tungsten</v>
       </c>
       <c r="B15" s="6">
         <f>Materials!D15/2</f>
-        <v>28</v>
+        <v>20.25</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -3388,11 +3436,11 @@
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="str">
         <f>Materials!A16</f>
-        <v>Bronze</v>
+        <v>Stainless Steel</v>
       </c>
       <c r="B16" s="6">
         <f>Materials!D16/2</f>
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -3408,13 +3456,13 @@
       <c r="N16" s="5"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
+      <c r="A17" s="2" t="str">
         <f>Materials!A17</f>
-        <v>0</v>
+        <v>Bronze</v>
       </c>
       <c r="B17" s="6">
         <f>Materials!D17/2</f>
-        <v>0</v>
+        <v>15.25</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>

</xml_diff>

<commit_message>
color changes and steel changes
</commit_message>
<xml_diff>
--- a/Info/balancing/metal system.xlsx
+++ b/Info/balancing/metal system.xlsx
@@ -593,7 +593,7 @@
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -703,23 +703,29 @@
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="3">
-        <v>7.8</v>
-      </c>
-      <c r="C4" s="3">
-        <v>4.25</v>
-      </c>
-      <c r="D4" s="3">
-        <v>20</v>
-      </c>
-      <c r="E4" s="3">
-        <v>6.21</v>
-      </c>
-      <c r="F4" s="3">
-        <v>250</v>
-      </c>
-      <c r="G4" s="3">
-        <v>400</v>
+      <c r="B4" s="9">
+        <f>(B2*2)*0.75</f>
+        <v>11.811</v>
+      </c>
+      <c r="C4" s="9">
+        <f t="shared" ref="C4:G4" si="0">(C2*2)*0.75</f>
+        <v>6</v>
+      </c>
+      <c r="D4" s="9">
+        <f t="shared" si="0"/>
+        <v>42.75</v>
+      </c>
+      <c r="E4" s="9">
+        <f t="shared" si="0"/>
+        <v>1.56</v>
+      </c>
+      <c r="F4" s="9">
+        <f t="shared" si="0"/>
+        <v>195</v>
+      </c>
+      <c r="G4" s="9">
+        <f t="shared" si="0"/>
+        <v>300</v>
       </c>
       <c r="H4" s="3">
         <v>1425</v>
@@ -1041,27 +1047,27 @@
       </c>
       <c r="B16" s="9">
         <f>B4+B7</f>
-        <v>14.99</v>
+        <v>19.001000000000001</v>
       </c>
       <c r="C16" s="9">
-        <f t="shared" ref="C16:G16" si="0">C4+C7</f>
-        <v>12.75</v>
+        <f t="shared" ref="C16:G16" si="1">C4+C7</f>
+        <v>14.5</v>
       </c>
       <c r="D16" s="9">
-        <f t="shared" si="0"/>
-        <v>56</v>
+        <f t="shared" si="1"/>
+        <v>78.75</v>
       </c>
       <c r="E16" s="9">
-        <f t="shared" si="0"/>
-        <v>11.309999999999999</v>
+        <f t="shared" si="1"/>
+        <v>6.66</v>
       </c>
       <c r="F16" s="9">
-        <f t="shared" si="0"/>
-        <v>410</v>
+        <f t="shared" si="1"/>
+        <v>355</v>
       </c>
       <c r="G16" s="9">
-        <f t="shared" si="0"/>
-        <v>680</v>
+        <f t="shared" si="1"/>
+        <v>580</v>
       </c>
       <c r="H16" s="9">
         <f>AVERAGE(H4,H7)</f>
@@ -1081,23 +1087,23 @@
         <v>16.22</v>
       </c>
       <c r="C17" s="9">
-        <f t="shared" ref="C17:G17" si="1">C3+C8</f>
+        <f t="shared" ref="C17:G17" si="2">C3+C8</f>
         <v>4.5</v>
       </c>
       <c r="D17" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>64</v>
       </c>
       <c r="E17" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14.68</v>
       </c>
       <c r="F17" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>79</v>
       </c>
       <c r="G17" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>239</v>
       </c>
       <c r="H17" s="8">
@@ -1118,23 +1124,23 @@
         <v>15.064</v>
       </c>
       <c r="C18" s="3">
-        <f t="shared" ref="C18:G18" si="2">C2+C7</f>
+        <f t="shared" ref="C18:G18" si="3">C2+C7</f>
         <v>12.5</v>
       </c>
       <c r="D18" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>64.5</v>
       </c>
       <c r="E18" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6.14</v>
       </c>
       <c r="F18" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>290</v>
       </c>
       <c r="G18" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>480</v>
       </c>
       <c r="H18" s="3">
@@ -1155,23 +1161,23 @@
         <v>19.43</v>
       </c>
       <c r="C19" s="3">
-        <f t="shared" ref="C19:G19" si="3">C9+C3</f>
+        <f t="shared" ref="C19:G19" si="4">C9+C3</f>
         <v>5.75</v>
       </c>
       <c r="D19" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>27.5</v>
       </c>
       <c r="E19" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>12.280000000000001</v>
       </c>
       <c r="F19" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>125</v>
       </c>
       <c r="G19" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>580</v>
       </c>
       <c r="H19" s="3">
@@ -1192,23 +1198,23 @@
         <v>28.189999999999998</v>
       </c>
       <c r="C20" s="9">
-        <f t="shared" ref="C20:G20" si="4">C15+C3</f>
+        <f t="shared" ref="C20:G20" si="5">C15+C3</f>
         <v>10.5</v>
       </c>
       <c r="D20" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>57.5</v>
       </c>
       <c r="E20" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7.8000000000000007</v>
       </c>
       <c r="F20" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>570</v>
       </c>
       <c r="G20" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1220</v>
       </c>
       <c r="H20" s="8">
@@ -1229,31 +1235,31 @@
         <v>13.41</v>
       </c>
       <c r="C21" s="3">
-        <f t="shared" ref="C21:I21" si="5">(C3*2)*0.75</f>
+        <f t="shared" ref="C21:I21" si="6">(C3*2)*0.75</f>
         <v>4.5</v>
       </c>
       <c r="D21" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>25.5</v>
       </c>
       <c r="E21" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>8.9700000000000006</v>
       </c>
       <c r="F21" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>105</v>
       </c>
       <c r="G21" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>330</v>
       </c>
       <c r="H21" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1626</v>
       </c>
       <c r="I21" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3843</v>
       </c>
     </row>
@@ -1570,55 +1576,55 @@
       </c>
       <c r="B4" s="6">
         <f>((Materials!D4/2)+Materials!B4)</f>
-        <v>17.8</v>
+        <v>33.186</v>
       </c>
       <c r="C4" s="5">
         <f>(Materials!G4/Materials!D4)+2</f>
-        <v>22</v>
+        <v>9.0175438596491233</v>
       </c>
       <c r="D4" s="5">
         <f>(Materials!B4*Materials!C4)+Materials!F4</f>
-        <v>283.14999999999998</v>
+        <v>265.86599999999999</v>
       </c>
       <c r="E4" s="5">
         <f>(Materials!B4*Materials!C4)*Materials!D4</f>
-        <v>663</v>
+        <v>3029.5214999999998</v>
       </c>
       <c r="F4" s="5">
         <f>((Materials!B4*Materials!C4)/2)+5</f>
-        <v>21.574999999999999</v>
+        <v>40.433</v>
       </c>
       <c r="G4" s="6">
         <f>Materials!D4/Materials!C4</f>
-        <v>4.7058823529411766</v>
+        <v>7.125</v>
       </c>
       <c r="H4" s="5">
         <f>60+Materials!D4</f>
-        <v>80</v>
+        <v>102.75</v>
       </c>
       <c r="I4" s="6">
         <f>Materials!G4/Materials!D4</f>
-        <v>20</v>
+        <v>7.0175438596491224</v>
       </c>
       <c r="J4" s="5">
         <f>Materials!G4*Materials!E4</f>
-        <v>2484</v>
+        <v>468</v>
       </c>
       <c r="K4" s="5">
         <f>Materials!E4+Materials!C4</f>
-        <v>10.46</v>
+        <v>7.5600000000000005</v>
       </c>
       <c r="L4" s="5">
         <f>Materials!E4+Materials!B4</f>
-        <v>14.01</v>
+        <v>13.371</v>
       </c>
       <c r="M4" s="5">
         <f t="shared" si="0"/>
-        <v>70.05</v>
+        <v>66.855000000000004</v>
       </c>
       <c r="N4" s="5">
         <f t="shared" si="1"/>
-        <v>24840</v>
+        <v>4680</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -2266,55 +2272,55 @@
       </c>
       <c r="B16" s="6">
         <f>((Materials!D16/2)+Materials!B16)</f>
-        <v>42.99</v>
+        <v>58.376000000000005</v>
       </c>
       <c r="C16" s="5">
         <f>(Materials!G16/Materials!D16)+2</f>
-        <v>14.142857142857142</v>
+        <v>9.3650793650793638</v>
       </c>
       <c r="D16" s="5">
         <f>(Materials!B16*Materials!C16)+Materials!F16</f>
-        <v>601.12249999999995</v>
+        <v>630.5145</v>
       </c>
       <c r="E16" s="5">
         <f>(Materials!B16*Materials!C16)*Materials!D16</f>
-        <v>10702.86</v>
+        <v>21696.766875000001</v>
       </c>
       <c r="F16" s="5">
         <f>((Materials!B16*Materials!C16)/2)+5</f>
-        <v>100.56125</v>
+        <v>142.75725</v>
       </c>
       <c r="G16" s="6">
         <f>Materials!D16/Materials!C16</f>
-        <v>4.3921568627450984</v>
+        <v>5.431034482758621</v>
       </c>
       <c r="H16" s="5">
         <f>60+Materials!D16</f>
-        <v>116</v>
+        <v>138.75</v>
       </c>
       <c r="I16" s="6">
         <f>Materials!G16/Materials!D16</f>
-        <v>12.142857142857142</v>
+        <v>7.3650793650793647</v>
       </c>
       <c r="J16" s="5">
         <f>Materials!G16*Materials!E16</f>
-        <v>7690.7999999999993</v>
+        <v>3862.8</v>
       </c>
       <c r="K16" s="5">
         <f>Materials!E16+Materials!C16</f>
-        <v>24.06</v>
+        <v>21.16</v>
       </c>
       <c r="L16" s="5">
         <f>Materials!E16+Materials!B16</f>
-        <v>26.299999999999997</v>
+        <v>25.661000000000001</v>
       </c>
       <c r="M16" s="5">
         <f t="shared" si="0"/>
-        <v>131.5</v>
+        <v>128.30500000000001</v>
       </c>
       <c r="N16" s="5">
         <f t="shared" si="1"/>
-        <v>76908</v>
+        <v>38628</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
@@ -2883,11 +2889,11 @@
       </c>
       <c r="B4" s="6">
         <f>Materials!D4/2</f>
-        <v>10</v>
+        <v>21.375</v>
       </c>
       <c r="C4" s="5">
         <f>Materials!G4+Materials!B4+Materials!C4+Materials!D4+Materials!E4</f>
-        <v>438.26</v>
+        <v>362.12099999999998</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -3183,11 +3189,11 @@
       </c>
       <c r="B16" s="6">
         <f>Materials!D16/2</f>
-        <v>28</v>
+        <v>39.375</v>
       </c>
       <c r="C16" s="5">
         <f>Materials!G16+Materials!B16+Materials!C16+Materials!D16+Materials!E16</f>
-        <v>775.05</v>
+        <v>698.91099999999994</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>

</xml_diff>

<commit_message>
Balancing and final preps for release
</commit_message>
<xml_diff>
--- a/Info/balancing/metal system.xlsx
+++ b/Info/balancing/metal system.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Materials" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>Density</t>
   </si>
@@ -156,6 +156,9 @@
   </si>
   <si>
     <t>Power Usage</t>
+  </si>
+  <si>
+    <t>Copilinvar-Tungstate</t>
   </si>
 </sst>
 </file>
@@ -592,13 +595,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{028B0D2B-13D9-4234-8CF2-6AB8658F4FDF}">
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22:I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
@@ -1264,15 +1267,41 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
+      <c r="A22" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="9">
+        <f>B20+B18</f>
+        <v>43.253999999999998</v>
+      </c>
+      <c r="C22" s="9">
+        <f t="shared" ref="C22:G22" si="7">C20+C18</f>
+        <v>23</v>
+      </c>
+      <c r="D22" s="9">
+        <f t="shared" si="7"/>
+        <v>122</v>
+      </c>
+      <c r="E22" s="9">
+        <f t="shared" si="7"/>
+        <v>13.940000000000001</v>
+      </c>
+      <c r="F22" s="9">
+        <f t="shared" si="7"/>
+        <v>860</v>
+      </c>
+      <c r="G22" s="9">
+        <f t="shared" si="7"/>
+        <v>1700</v>
+      </c>
+      <c r="H22" s="8">
+        <f>AVERAGE(H20,H18)</f>
+        <v>1976</v>
+      </c>
+      <c r="I22" s="8">
+        <f>AVERAGE(I20,I18)</f>
+        <v>3273.5</v>
+      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
@@ -1382,8 +1411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21:N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1561,11 +1590,11 @@
         <v>14.92</v>
       </c>
       <c r="M3" s="5">
-        <f t="shared" ref="M3:M21" si="0">L3*5</f>
+        <f t="shared" ref="M3:M22" si="0">L3*5</f>
         <v>74.599999999999994</v>
       </c>
       <c r="N3" s="5">
-        <f t="shared" ref="N3:N21" si="1">J3*10</f>
+        <f t="shared" ref="N3:N22" si="1">J3*10</f>
         <v>13156.000000000002</v>
       </c>
     </row>
@@ -2614,20 +2643,62 @@
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="5"/>
-      <c r="N22" s="5"/>
+      <c r="A22" s="2" t="str">
+        <f>Materials!A22</f>
+        <v>Copilinvar-Tungstate</v>
+      </c>
+      <c r="B22" s="6">
+        <f>((Materials!D22/2)+Materials!B22)</f>
+        <v>104.25399999999999</v>
+      </c>
+      <c r="C22" s="5">
+        <f>(Materials!G22/Materials!D22)+2</f>
+        <v>15.934426229508198</v>
+      </c>
+      <c r="D22" s="5">
+        <f>(Materials!B22*Materials!C22)+Materials!F22</f>
+        <v>1854.8420000000001</v>
+      </c>
+      <c r="E22" s="5">
+        <f>(Materials!B22*Materials!C22)*Materials!D22</f>
+        <v>121370.724</v>
+      </c>
+      <c r="F22" s="5">
+        <f>((Materials!B22*Materials!C22)/2)+5</f>
+        <v>502.42099999999999</v>
+      </c>
+      <c r="G22" s="6">
+        <f>Materials!D22/Materials!C22</f>
+        <v>5.3043478260869561</v>
+      </c>
+      <c r="H22" s="5">
+        <f>60+Materials!D22</f>
+        <v>182</v>
+      </c>
+      <c r="I22" s="6">
+        <f>Materials!G22/Materials!D22</f>
+        <v>13.934426229508198</v>
+      </c>
+      <c r="J22" s="5">
+        <f>Materials!G22*Materials!E22</f>
+        <v>23698.000000000004</v>
+      </c>
+      <c r="K22" s="5">
+        <f>Materials!E22+Materials!C22</f>
+        <v>36.94</v>
+      </c>
+      <c r="L22" s="5">
+        <f>Materials!E22+Materials!B22</f>
+        <v>57.194000000000003</v>
+      </c>
+      <c r="M22" s="5">
+        <f t="shared" si="0"/>
+        <v>285.97000000000003</v>
+      </c>
+      <c r="N22" s="5">
+        <f t="shared" si="1"/>
+        <v>236980.00000000003</v>
+      </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
@@ -2784,7 +2855,7 @@
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C21"/>
+      <selection activeCell="C21" sqref="C21:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3333,12 +3404,18 @@
       <c r="N21" s="5"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
+      <c r="A22" s="2" t="str">
         <f>Materials!A22</f>
-        <v>0</v>
-      </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="5"/>
+        <v>Copilinvar-Tungstate</v>
+      </c>
+      <c r="B22" s="6">
+        <f>Materials!D22/2</f>
+        <v>61</v>
+      </c>
+      <c r="C22" s="5">
+        <f>Materials!G22+Materials!B22+Materials!C22+Materials!D22+Materials!E22</f>
+        <v>1902.194</v>
+      </c>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
@@ -3352,10 +3429,7 @@
       <c r="N22" s="5"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
-        <f>Materials!A23</f>
-        <v>0</v>
-      </c>
+      <c r="A23" s="2"/>
       <c r="B23" s="6"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -3371,10 +3445,7 @@
       <c r="N23" s="5"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
-        <f>Materials!A24</f>
-        <v>0</v>
-      </c>
+      <c r="A24" s="2"/>
       <c r="B24" s="6"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
@@ -3390,10 +3461,7 @@
       <c r="N24" s="5"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
-        <f>Materials!A25</f>
-        <v>0</v>
-      </c>
+      <c r="A25" s="2"/>
       <c r="B25" s="6"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
@@ -3409,10 +3477,7 @@
       <c r="N25" s="5"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
-        <f>Materials!A26</f>
-        <v>0</v>
-      </c>
+      <c r="A26" s="2"/>
       <c r="B26" s="6"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
@@ -3428,10 +3493,7 @@
       <c r="N26" s="5"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
-        <f>Materials!A27</f>
-        <v>0</v>
-      </c>
+      <c r="A27" s="2"/>
       <c r="B27" s="6"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
@@ -3447,10 +3509,7 @@
       <c r="N27" s="5"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
-        <f>Materials!A28</f>
-        <v>0</v>
-      </c>
+      <c r="A28" s="2"/>
       <c r="B28" s="6"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
@@ -3466,10 +3525,7 @@
       <c r="N28" s="5"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
-        <f>Materials!A29</f>
-        <v>0</v>
-      </c>
+      <c r="A29" s="2"/>
       <c r="B29" s="6"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
@@ -3485,10 +3541,7 @@
       <c r="N29" s="5"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
-        <f>Materials!A30</f>
-        <v>0</v>
-      </c>
+      <c r="A30" s="2"/>
       <c r="B30" s="6"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
@@ -3504,10 +3557,7 @@
       <c r="N30" s="5"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
-        <f>Materials!A31</f>
-        <v>0</v>
-      </c>
+      <c r="A31" s="2"/>
       <c r="B31" s="6"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>

</xml_diff>

<commit_message>
graphics, alloys and more
</commit_message>
<xml_diff>
--- a/Info/balancing/metal system.xlsx
+++ b/Info/balancing/metal system.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Density</t>
   </si>
@@ -137,9 +137,6 @@
     <t>Mining Speed</t>
   </si>
   <si>
-    <t>Cadmium</t>
-  </si>
-  <si>
     <t>Tungsten</t>
   </si>
   <si>
@@ -158,7 +155,16 @@
     <t>Power Usage</t>
   </si>
   <si>
-    <t>Copilinvar-Tungstate</t>
+    <t>Stainless-Copilinvar-Tungstate</t>
+  </si>
+  <si>
+    <t>Aluminium</t>
+  </si>
+  <si>
+    <t>Nickel</t>
+  </si>
+  <si>
+    <t>Zinc</t>
   </si>
 </sst>
 </file>
@@ -277,7 +283,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -307,6 +313,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -596,12 +605,12 @@
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22:I22"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
@@ -988,36 +997,36 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="B14" s="3">
-        <v>8.65</v>
+        <v>7.14</v>
       </c>
       <c r="C14" s="3">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="D14" s="3">
-        <v>4.5999999999999996</v>
+        <v>12</v>
       </c>
       <c r="E14" s="3">
-        <v>1.46</v>
+        <v>11.6</v>
       </c>
       <c r="F14" s="3">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="G14" s="3">
-        <v>78</v>
+        <v>108</v>
       </c>
       <c r="H14" s="3">
-        <v>321</v>
+        <v>419</v>
       </c>
       <c r="I14" s="3">
-        <v>767</v>
+        <v>907</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B15" s="9">
         <v>19.25</v>
@@ -1046,284 +1055,320 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="9">
+        <v>2.7</v>
+      </c>
+      <c r="C16" s="9">
+        <v>2.75</v>
+      </c>
+      <c r="D16" s="9">
+        <v>10</v>
+      </c>
+      <c r="E16" s="9">
+        <v>2.37</v>
+      </c>
+      <c r="F16" s="9">
+        <v>26</v>
+      </c>
+      <c r="G16" s="9">
+        <v>70</v>
+      </c>
+      <c r="H16" s="9">
+        <v>660</v>
+      </c>
+      <c r="I16" s="9">
+        <v>2470</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="9">
+        <v>8.9090000000000007</v>
+      </c>
+      <c r="C17" s="9">
+        <v>4</v>
+      </c>
+      <c r="D17" s="9">
+        <v>31</v>
+      </c>
+      <c r="E17" s="9">
+        <v>9.09</v>
+      </c>
+      <c r="F17" s="9">
+        <v>76</v>
+      </c>
+      <c r="G17" s="9">
+        <v>200</v>
+      </c>
+      <c r="H17" s="8">
+        <v>1455</v>
+      </c>
+      <c r="I17" s="8">
+        <v>2730</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="9">
-        <f>B4+B7</f>
+      <c r="B18" s="9">
+        <f t="shared" ref="B18:F18" si="1">B4+B7</f>
         <v>19.001000000000001</v>
       </c>
-      <c r="C16" s="9">
-        <f t="shared" ref="C16:G16" si="1">C4+C7</f>
+      <c r="C18" s="9">
+        <f t="shared" si="1"/>
         <v>14.5</v>
       </c>
-      <c r="D16" s="9">
-        <f t="shared" si="1"/>
+      <c r="D18" s="9">
+        <f>D4+D7</f>
         <v>78.75</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E18" s="9">
         <f t="shared" si="1"/>
         <v>6.66</v>
       </c>
-      <c r="F16" s="9">
+      <c r="F18" s="9">
         <f t="shared" si="1"/>
         <v>355</v>
       </c>
-      <c r="G16" s="9">
-        <f t="shared" si="1"/>
+      <c r="G18" s="9">
+        <f>G4+G7</f>
         <v>580</v>
       </c>
-      <c r="H16" s="9">
+      <c r="H18" s="9">
         <f>AVERAGE(H4,H7)</f>
         <v>1642.5</v>
       </c>
-      <c r="I16" s="9">
+      <c r="I18" s="9">
         <f>AVERAGE(I4,I7)</f>
         <v>2766</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="9">
+      <c r="B19" s="9">
         <f>B3+B8</f>
         <v>16.22</v>
       </c>
-      <c r="C17" s="9">
-        <f t="shared" ref="C17:G17" si="2">C3+C8</f>
+      <c r="C19" s="9">
+        <f t="shared" ref="C19:G19" si="2">C3+C8</f>
         <v>4.5</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D19" s="9">
         <f t="shared" si="2"/>
         <v>64</v>
       </c>
-      <c r="E17" s="9">
+      <c r="E19" s="9">
         <f t="shared" si="2"/>
         <v>14.68</v>
       </c>
-      <c r="F17" s="9">
+      <c r="F19" s="9">
         <f t="shared" si="2"/>
         <v>79</v>
       </c>
-      <c r="G17" s="9">
+      <c r="G19" s="9">
         <f t="shared" si="2"/>
         <v>239</v>
       </c>
-      <c r="H17" s="8">
+      <c r="H19" s="8">
         <f>AVERAGE(H3,H8)</f>
         <v>658</v>
       </c>
-      <c r="I17" s="8">
+      <c r="I19" s="8">
         <f>AVERAGE(I3,I8)</f>
         <v>2581</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="9">
+        <f>B2+B7+B17</f>
+        <v>23.972999999999999</v>
+      </c>
+      <c r="C20" s="9">
+        <f t="shared" ref="C20:G20" si="3">C2+C7+C17</f>
+        <v>16.5</v>
+      </c>
+      <c r="D20" s="9">
+        <f t="shared" si="3"/>
+        <v>95.5</v>
+      </c>
+      <c r="E20" s="9">
+        <f t="shared" si="3"/>
+        <v>15.23</v>
+      </c>
+      <c r="F20" s="9">
+        <f t="shared" si="3"/>
+        <v>366</v>
+      </c>
+      <c r="G20" s="9">
+        <f t="shared" si="3"/>
+        <v>680</v>
+      </c>
+      <c r="H20" s="8">
+        <f>AVERAGE(H17,H7,H2)</f>
+        <v>1617.6666666666667</v>
+      </c>
+      <c r="I20" s="8">
+        <f>AVERAGE(I17,I7,I2)</f>
+        <v>2754</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="3">
-        <f>B2+B7</f>
-        <v>15.064</v>
-      </c>
-      <c r="C18" s="3">
-        <f t="shared" ref="C18:G18" si="3">C2+C7</f>
-        <v>12.5</v>
-      </c>
-      <c r="D18" s="3">
-        <f t="shared" si="3"/>
-        <v>64.5</v>
-      </c>
-      <c r="E18" s="3">
-        <f t="shared" si="3"/>
-        <v>6.14</v>
-      </c>
-      <c r="F18" s="3">
-        <f t="shared" si="3"/>
-        <v>290</v>
-      </c>
-      <c r="G18" s="3">
-        <f t="shared" si="3"/>
-        <v>480</v>
-      </c>
-      <c r="H18" s="3">
-        <f>AVERAGE(H2,H7)</f>
-        <v>1699</v>
-      </c>
-      <c r="I18" s="3">
-        <f>AVERAGE(I2,I7)</f>
-        <v>2766</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B19" s="3">
-        <f>B9+B3</f>
+      <c r="B21" s="3">
+        <f>B3+B9</f>
         <v>19.43</v>
       </c>
-      <c r="C19" s="3">
-        <f t="shared" ref="C19:G19" si="4">C9+C3</f>
+      <c r="C21" s="3">
+        <f t="shared" ref="C21:G21" si="4">C3+C9</f>
         <v>5.75</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D21" s="3">
         <f t="shared" si="4"/>
         <v>27.5</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E21" s="3">
         <f t="shared" si="4"/>
         <v>12.280000000000001</v>
       </c>
-      <c r="F19" s="3">
+      <c r="F21" s="3">
         <f t="shared" si="4"/>
         <v>125</v>
       </c>
-      <c r="G19" s="3">
+      <c r="G21" s="3">
         <f t="shared" si="4"/>
         <v>580</v>
       </c>
-      <c r="H19" s="3">
+      <c r="H21" s="3">
         <f>AVERAGE(H3,H9)</f>
         <v>1022.5</v>
       </c>
-      <c r="I19" s="3">
+      <c r="I21" s="3">
         <f>AVERAGE(I3,I9)</f>
         <v>2387</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" s="9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="9">
         <f>B15+B3</f>
         <v>28.189999999999998</v>
       </c>
-      <c r="C20" s="9">
-        <f t="shared" ref="C20:G20" si="5">C15+C3</f>
+      <c r="C22" s="9">
+        <f t="shared" ref="C22:G22" si="5">C15+C3</f>
         <v>10.5</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D22" s="9">
         <f t="shared" si="5"/>
         <v>57.5</v>
       </c>
-      <c r="E20" s="9">
+      <c r="E22" s="9">
         <f t="shared" si="5"/>
         <v>7.8000000000000007</v>
       </c>
-      <c r="F20" s="9">
+      <c r="F22" s="9">
         <f t="shared" si="5"/>
         <v>570</v>
       </c>
-      <c r="G20" s="9">
+      <c r="G22" s="9">
         <f t="shared" si="5"/>
         <v>1220</v>
       </c>
-      <c r="H20" s="8">
+      <c r="H22" s="8">
         <f>AVERAGE(H15,H3)</f>
         <v>2253</v>
       </c>
-      <c r="I20" s="8">
-        <f>AVERAGE(I15,I3)</f>
-        <v>3781</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B21" s="3">
+      <c r="I22" s="8">
+        <f>AVERAGE(I17,I5)</f>
+        <v>2730</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="3">
         <f>(B3*2)*0.75</f>
         <v>13.41</v>
       </c>
-      <c r="C21" s="3">
-        <f t="shared" ref="C21:I21" si="6">(C3*2)*0.75</f>
+      <c r="C23" s="3">
+        <f t="shared" ref="C23:I23" si="6">(C3*2)*0.75</f>
         <v>4.5</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D23" s="3">
         <f t="shared" si="6"/>
         <v>25.5</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E23" s="3">
         <f t="shared" si="6"/>
         <v>8.9700000000000006</v>
       </c>
-      <c r="F21" s="3">
+      <c r="F23" s="3">
         <f t="shared" si="6"/>
         <v>105</v>
       </c>
-      <c r="G21" s="3">
+      <c r="G23" s="3">
         <f t="shared" si="6"/>
         <v>330</v>
       </c>
-      <c r="H21" s="3">
+      <c r="H23" s="3">
         <f t="shared" si="6"/>
         <v>1626</v>
       </c>
-      <c r="I21" s="3">
+      <c r="I23" s="3">
         <f t="shared" si="6"/>
         <v>3843</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B22" s="9">
-        <f>B20+B18</f>
-        <v>43.253999999999998</v>
-      </c>
-      <c r="C22" s="9">
-        <f t="shared" ref="C22:G22" si="7">C20+C18</f>
-        <v>23</v>
-      </c>
-      <c r="D22" s="9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="9">
+        <f>B18+B20+B22</f>
+        <v>71.164000000000001</v>
+      </c>
+      <c r="C24" s="9">
+        <f t="shared" ref="C24:I24" si="7">C18+C20+C22</f>
+        <v>41.5</v>
+      </c>
+      <c r="D24" s="9">
         <f t="shared" si="7"/>
-        <v>122</v>
-      </c>
-      <c r="E22" s="9">
+        <v>231.75</v>
+      </c>
+      <c r="E24" s="9">
         <f t="shared" si="7"/>
-        <v>13.940000000000001</v>
-      </c>
-      <c r="F22" s="9">
+        <v>29.69</v>
+      </c>
+      <c r="F24" s="9">
         <f t="shared" si="7"/>
-        <v>860</v>
-      </c>
-      <c r="G22" s="9">
+        <v>1291</v>
+      </c>
+      <c r="G24" s="9">
         <f t="shared" si="7"/>
-        <v>1700</v>
-      </c>
-      <c r="H22" s="8">
-        <f>AVERAGE(H20,H18)</f>
-        <v>1976</v>
-      </c>
-      <c r="I22" s="8">
-        <f>AVERAGE(I20,I18)</f>
-        <v>3273.5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
+        <v>2480</v>
+      </c>
+      <c r="H24" s="8">
+        <f>AVERAGE(H18,H20,H22)</f>
+        <v>1837.7222222222224</v>
+      </c>
+      <c r="I24" s="8">
+        <f>AVERAGE(I18,I20,I22)</f>
+        <v>2750</v>
+      </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
@@ -1404,6 +1449,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1412,12 +1458,12 @@
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21:N22"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.28515625" style="4" bestFit="1" customWidth="1"/>
@@ -1590,11 +1636,11 @@
         <v>14.92</v>
       </c>
       <c r="M3" s="5">
-        <f t="shared" ref="M3:M22" si="0">L3*5</f>
+        <f t="shared" ref="M3:M24" si="0">L3*5</f>
         <v>74.599999999999994</v>
       </c>
       <c r="N3" s="5">
-        <f t="shared" ref="N3:N22" si="1">J3*10</f>
+        <f t="shared" ref="N3:N24" si="1">J3*10</f>
         <v>13156.000000000002</v>
       </c>
     </row>
@@ -2181,59 +2227,59 @@
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="str">
         <f>Materials!A14</f>
-        <v>Cadmium</v>
+        <v>Zinc</v>
       </c>
       <c r="B14" s="6">
         <f>((Materials!D14/2)+Materials!B14)</f>
-        <v>10.95</v>
+        <v>13.14</v>
       </c>
       <c r="C14" s="5">
         <f>(Materials!G14/Materials!D14)+2</f>
-        <v>18.956521739130437</v>
+        <v>11</v>
       </c>
       <c r="D14" s="5">
         <f>(Materials!B14*Materials!C14)+Materials!F14</f>
-        <v>42.3</v>
+        <v>60.849999999999994</v>
       </c>
       <c r="E14" s="5">
         <f>(Materials!B14*Materials!C14)*Materials!D14</f>
-        <v>79.58</v>
+        <v>214.2</v>
       </c>
       <c r="F14" s="5">
         <f>((Materials!B14*Materials!C14)/2)+5</f>
-        <v>13.65</v>
+        <v>13.924999999999999</v>
       </c>
       <c r="G14" s="6">
         <f>Materials!D14/Materials!C14</f>
-        <v>2.2999999999999998</v>
+        <v>4.8</v>
       </c>
       <c r="H14" s="5">
         <f>60+Materials!D14</f>
-        <v>64.599999999999994</v>
+        <v>72</v>
       </c>
       <c r="I14" s="6">
         <f>Materials!G14/Materials!D14</f>
-        <v>16.956521739130437</v>
+        <v>9</v>
       </c>
       <c r="J14" s="5">
         <f>Materials!G14*Materials!E14</f>
-        <v>113.88</v>
+        <v>1252.8</v>
       </c>
       <c r="K14" s="5">
         <f>Materials!E14+Materials!C14</f>
-        <v>3.46</v>
+        <v>14.1</v>
       </c>
       <c r="L14" s="5">
         <f>Materials!E14+Materials!B14</f>
-        <v>10.11</v>
+        <v>18.739999999999998</v>
       </c>
       <c r="M14" s="5">
         <f t="shared" si="0"/>
-        <v>50.55</v>
+        <v>93.699999999999989</v>
       </c>
       <c r="N14" s="5">
         <f t="shared" si="1"/>
-        <v>1138.8</v>
+        <v>12528</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -2297,440 +2343,524 @@
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="str">
         <f>Materials!A16</f>
-        <v>Stainless Steel</v>
+        <v>Aluminium</v>
       </c>
       <c r="B16" s="6">
         <f>((Materials!D16/2)+Materials!B16)</f>
-        <v>58.376000000000005</v>
+        <v>7.7</v>
       </c>
       <c r="C16" s="5">
         <f>(Materials!G16/Materials!D16)+2</f>
-        <v>9.3650793650793638</v>
+        <v>9</v>
       </c>
       <c r="D16" s="5">
         <f>(Materials!B16*Materials!C16)+Materials!F16</f>
-        <v>630.5145</v>
+        <v>33.424999999999997</v>
       </c>
       <c r="E16" s="5">
         <f>(Materials!B16*Materials!C16)*Materials!D16</f>
-        <v>21696.766875000001</v>
+        <v>74.25</v>
       </c>
       <c r="F16" s="5">
         <f>((Materials!B16*Materials!C16)/2)+5</f>
-        <v>142.75725</v>
+        <v>8.7125000000000004</v>
       </c>
       <c r="G16" s="6">
         <f>Materials!D16/Materials!C16</f>
-        <v>5.431034482758621</v>
+        <v>3.6363636363636362</v>
       </c>
       <c r="H16" s="5">
         <f>60+Materials!D16</f>
-        <v>138.75</v>
+        <v>70</v>
       </c>
       <c r="I16" s="6">
         <f>Materials!G16/Materials!D16</f>
-        <v>7.3650793650793647</v>
+        <v>7</v>
       </c>
       <c r="J16" s="5">
         <f>Materials!G16*Materials!E16</f>
-        <v>3862.8</v>
+        <v>165.9</v>
       </c>
       <c r="K16" s="5">
         <f>Materials!E16+Materials!C16</f>
-        <v>21.16</v>
+        <v>5.12</v>
       </c>
       <c r="L16" s="5">
         <f>Materials!E16+Materials!B16</f>
-        <v>25.661000000000001</v>
+        <v>5.07</v>
       </c>
       <c r="M16" s="5">
         <f t="shared" si="0"/>
-        <v>128.30500000000001</v>
+        <v>25.35</v>
       </c>
       <c r="N16" s="5">
         <f t="shared" si="1"/>
-        <v>38628</v>
+        <v>1659</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="str">
         <f>Materials!A17</f>
-        <v>Bronze</v>
+        <v>Nickel</v>
       </c>
       <c r="B17" s="6">
         <f>((Materials!D17/2)+Materials!B17)</f>
-        <v>48.22</v>
+        <v>24.408999999999999</v>
       </c>
       <c r="C17" s="5">
         <f>(Materials!G17/Materials!D17)+2</f>
-        <v>5.734375</v>
+        <v>8.4516129032258061</v>
       </c>
       <c r="D17" s="5">
         <f>(Materials!B17*Materials!C17)+Materials!F17</f>
-        <v>151.99</v>
+        <v>111.636</v>
       </c>
       <c r="E17" s="5">
         <f>(Materials!B17*Materials!C17)*Materials!D17</f>
-        <v>4671.3599999999997</v>
+        <v>1104.7160000000001</v>
       </c>
       <c r="F17" s="5">
         <f>((Materials!B17*Materials!C17)/2)+5</f>
-        <v>41.494999999999997</v>
+        <v>22.818000000000001</v>
       </c>
       <c r="G17" s="6">
         <f>Materials!D17/Materials!C17</f>
-        <v>14.222222222222221</v>
+        <v>7.75</v>
       </c>
       <c r="H17" s="5">
         <f>60+Materials!D17</f>
-        <v>124</v>
+        <v>91</v>
       </c>
       <c r="I17" s="6">
         <f>Materials!G17/Materials!D17</f>
-        <v>3.734375</v>
+        <v>6.4516129032258061</v>
       </c>
       <c r="J17" s="5">
         <f>Materials!G17*Materials!E17</f>
-        <v>3508.52</v>
+        <v>1818</v>
       </c>
       <c r="K17" s="5">
         <f>Materials!E17+Materials!C17</f>
-        <v>19.18</v>
+        <v>13.09</v>
       </c>
       <c r="L17" s="5">
         <f>Materials!E17+Materials!B17</f>
-        <v>30.9</v>
+        <v>17.999000000000002</v>
       </c>
       <c r="M17" s="5">
         <f t="shared" si="0"/>
-        <v>154.5</v>
+        <v>89.995000000000005</v>
       </c>
       <c r="N17" s="5">
         <f t="shared" si="1"/>
-        <v>35085.199999999997</v>
+        <v>18180</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="str">
         <f>Materials!A18</f>
-        <v>Elinvar</v>
+        <v>Stainless Steel</v>
       </c>
       <c r="B18" s="6">
         <f>((Materials!D18/2)+Materials!B18)</f>
-        <v>47.314</v>
+        <v>58.376000000000005</v>
       </c>
       <c r="C18" s="5">
         <f>(Materials!G18/Materials!D18)+2</f>
-        <v>9.4418604651162781</v>
+        <v>9.3650793650793638</v>
       </c>
       <c r="D18" s="5">
         <f>(Materials!B18*Materials!C18)+Materials!F18</f>
-        <v>478.3</v>
+        <v>630.5145</v>
       </c>
       <c r="E18" s="5">
         <f>(Materials!B18*Materials!C18)*Materials!D18</f>
-        <v>12145.35</v>
+        <v>21696.766875000001</v>
       </c>
       <c r="F18" s="5">
         <f>((Materials!B18*Materials!C18)/2)+5</f>
-        <v>99.15</v>
+        <v>142.75725</v>
       </c>
       <c r="G18" s="6">
         <f>Materials!D18/Materials!C18</f>
-        <v>5.16</v>
+        <v>5.431034482758621</v>
       </c>
       <c r="H18" s="5">
         <f>60+Materials!D18</f>
-        <v>124.5</v>
+        <v>138.75</v>
       </c>
       <c r="I18" s="6">
         <f>Materials!G18/Materials!D18</f>
-        <v>7.441860465116279</v>
+        <v>7.3650793650793647</v>
       </c>
       <c r="J18" s="5">
         <f>Materials!G18*Materials!E18</f>
-        <v>2947.2</v>
+        <v>3862.8</v>
       </c>
       <c r="K18" s="5">
         <f>Materials!E18+Materials!C18</f>
-        <v>18.64</v>
+        <v>21.16</v>
       </c>
       <c r="L18" s="5">
         <f>Materials!E18+Materials!B18</f>
-        <v>21.204000000000001</v>
+        <v>25.661000000000001</v>
       </c>
       <c r="M18" s="5">
         <f t="shared" si="0"/>
-        <v>106.02000000000001</v>
+        <v>128.30500000000001</v>
       </c>
       <c r="N18" s="5">
         <f t="shared" si="1"/>
-        <v>29472</v>
+        <v>38628</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="str">
         <f>Materials!A19</f>
-        <v>Billon</v>
+        <v>Bronze</v>
       </c>
       <c r="B19" s="6">
         <f>((Materials!D19/2)+Materials!B19)</f>
-        <v>33.18</v>
+        <v>48.22</v>
       </c>
       <c r="C19" s="5">
         <f>(Materials!G19/Materials!D19)+2</f>
-        <v>23.09090909090909</v>
+        <v>5.734375</v>
       </c>
       <c r="D19" s="5">
         <f>(Materials!B19*Materials!C19)+Materials!F19</f>
-        <v>236.7225</v>
+        <v>151.99</v>
       </c>
       <c r="E19" s="5">
         <f>(Materials!B19*Materials!C19)*Materials!D19</f>
-        <v>3072.3687500000001</v>
+        <v>4671.3599999999997</v>
       </c>
       <c r="F19" s="5">
         <f>((Materials!B19*Materials!C19)/2)+5</f>
-        <v>60.861249999999998</v>
+        <v>41.494999999999997</v>
       </c>
       <c r="G19" s="6">
         <f>Materials!D19/Materials!C19</f>
-        <v>4.7826086956521738</v>
+        <v>14.222222222222221</v>
       </c>
       <c r="H19" s="5">
         <f>60+Materials!D19</f>
-        <v>87.5</v>
+        <v>124</v>
       </c>
       <c r="I19" s="6">
         <f>Materials!G19/Materials!D19</f>
-        <v>21.09090909090909</v>
+        <v>3.734375</v>
       </c>
       <c r="J19" s="5">
         <f>Materials!G19*Materials!E19</f>
-        <v>7122.4000000000005</v>
+        <v>3508.52</v>
       </c>
       <c r="K19" s="5">
         <f>Materials!E19+Materials!C19</f>
-        <v>18.03</v>
+        <v>19.18</v>
       </c>
       <c r="L19" s="5">
         <f>Materials!E19+Materials!B19</f>
-        <v>31.71</v>
+        <v>30.9</v>
       </c>
       <c r="M19" s="5">
         <f t="shared" si="0"/>
-        <v>158.55000000000001</v>
+        <v>154.5</v>
       </c>
       <c r="N19" s="5">
         <f t="shared" si="1"/>
-        <v>71224</v>
+        <v>35085.199999999997</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="str">
         <f>Materials!A20</f>
-        <v>Copper-Tungsten</v>
+        <v>Elinvar</v>
       </c>
       <c r="B20" s="6">
         <f>((Materials!D20/2)+Materials!B20)</f>
-        <v>56.94</v>
+        <v>71.722999999999999</v>
       </c>
       <c r="C20" s="5">
         <f>(Materials!G20/Materials!D20)+2</f>
-        <v>23.217391304347824</v>
+        <v>9.1204188481675388</v>
       </c>
       <c r="D20" s="5">
         <f>(Materials!B20*Materials!C20)+Materials!F20</f>
-        <v>865.995</v>
+        <v>761.55449999999996</v>
       </c>
       <c r="E20" s="5">
         <f>(Materials!B20*Materials!C20)*Materials!D20</f>
-        <v>17019.712500000001</v>
+        <v>37775.454749999997</v>
       </c>
       <c r="F20" s="5">
         <f>((Materials!B20*Materials!C20)/2)+5</f>
-        <v>152.9975</v>
+        <v>202.77724999999998</v>
       </c>
       <c r="G20" s="6">
         <f>Materials!D20/Materials!C20</f>
-        <v>5.4761904761904763</v>
+        <v>5.7878787878787881</v>
       </c>
       <c r="H20" s="5">
         <f>60+Materials!D20</f>
-        <v>117.5</v>
+        <v>155.5</v>
       </c>
       <c r="I20" s="6">
         <f>Materials!G20/Materials!D20</f>
-        <v>21.217391304347824</v>
+        <v>7.1204188481675397</v>
       </c>
       <c r="J20" s="5">
         <f>Materials!G20*Materials!E20</f>
-        <v>9516</v>
+        <v>10356.4</v>
       </c>
       <c r="K20" s="5">
         <f>Materials!E20+Materials!C20</f>
-        <v>18.3</v>
+        <v>31.73</v>
       </c>
       <c r="L20" s="5">
         <f>Materials!E20+Materials!B20</f>
-        <v>35.989999999999995</v>
+        <v>39.203000000000003</v>
       </c>
       <c r="M20" s="5">
         <f t="shared" si="0"/>
-        <v>179.95</v>
+        <v>196.01500000000001</v>
       </c>
       <c r="N20" s="5">
         <f t="shared" si="1"/>
-        <v>95160</v>
+        <v>103564</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="str">
         <f>Materials!A21</f>
-        <v>Copper-Hydride</v>
+        <v>Billon</v>
       </c>
       <c r="B21" s="6">
         <f>((Materials!D21/2)+Materials!B21)</f>
-        <v>26.16</v>
+        <v>33.18</v>
       </c>
       <c r="C21" s="5">
         <f>(Materials!G21/Materials!D21)+2</f>
-        <v>14.941176470588236</v>
+        <v>23.09090909090909</v>
       </c>
       <c r="D21" s="5">
         <f>(Materials!B21*Materials!C21)+Materials!F21</f>
-        <v>165.345</v>
+        <v>236.7225</v>
       </c>
       <c r="E21" s="5">
         <f>(Materials!B21*Materials!C21)*Materials!D21</f>
-        <v>1538.7974999999999</v>
+        <v>3072.3687500000001</v>
       </c>
       <c r="F21" s="5">
         <f>((Materials!B21*Materials!C21)/2)+5</f>
-        <v>35.172499999999999</v>
+        <v>60.861249999999998</v>
       </c>
       <c r="G21" s="6">
         <f>Materials!D21/Materials!C21</f>
-        <v>5.666666666666667</v>
+        <v>4.7826086956521738</v>
       </c>
       <c r="H21" s="5">
         <f>60+Materials!D21</f>
-        <v>85.5</v>
+        <v>87.5</v>
       </c>
       <c r="I21" s="6">
         <f>Materials!G21/Materials!D21</f>
-        <v>12.941176470588236</v>
+        <v>21.09090909090909</v>
       </c>
       <c r="J21" s="5">
         <f>Materials!G21*Materials!E21</f>
-        <v>2960.1000000000004</v>
+        <v>7122.4000000000005</v>
       </c>
       <c r="K21" s="5">
         <f>Materials!E21+Materials!C21</f>
-        <v>13.47</v>
+        <v>18.03</v>
       </c>
       <c r="L21" s="5">
         <f>Materials!E21+Materials!B21</f>
-        <v>22.380000000000003</v>
+        <v>31.71</v>
       </c>
       <c r="M21" s="5">
         <f t="shared" si="0"/>
-        <v>111.9</v>
+        <v>158.55000000000001</v>
       </c>
       <c r="N21" s="5">
         <f t="shared" si="1"/>
-        <v>29601.000000000004</v>
+        <v>71224</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="str">
         <f>Materials!A22</f>
-        <v>Copilinvar-Tungstate</v>
+        <v>Copper-Tungsten</v>
       </c>
       <c r="B22" s="6">
         <f>((Materials!D22/2)+Materials!B22)</f>
-        <v>104.25399999999999</v>
+        <v>56.94</v>
       </c>
       <c r="C22" s="5">
         <f>(Materials!G22/Materials!D22)+2</f>
-        <v>15.934426229508198</v>
+        <v>23.217391304347824</v>
       </c>
       <c r="D22" s="5">
         <f>(Materials!B22*Materials!C22)+Materials!F22</f>
-        <v>1854.8420000000001</v>
+        <v>865.995</v>
       </c>
       <c r="E22" s="5">
         <f>(Materials!B22*Materials!C22)*Materials!D22</f>
-        <v>121370.724</v>
+        <v>17019.712500000001</v>
       </c>
       <c r="F22" s="5">
         <f>((Materials!B22*Materials!C22)/2)+5</f>
-        <v>502.42099999999999</v>
+        <v>152.9975</v>
       </c>
       <c r="G22" s="6">
         <f>Materials!D22/Materials!C22</f>
-        <v>5.3043478260869561</v>
+        <v>5.4761904761904763</v>
       </c>
       <c r="H22" s="5">
         <f>60+Materials!D22</f>
-        <v>182</v>
+        <v>117.5</v>
       </c>
       <c r="I22" s="6">
         <f>Materials!G22/Materials!D22</f>
-        <v>13.934426229508198</v>
+        <v>21.217391304347824</v>
       </c>
       <c r="J22" s="5">
         <f>Materials!G22*Materials!E22</f>
-        <v>23698.000000000004</v>
+        <v>9516</v>
       </c>
       <c r="K22" s="5">
         <f>Materials!E22+Materials!C22</f>
-        <v>36.94</v>
+        <v>18.3</v>
       </c>
       <c r="L22" s="5">
         <f>Materials!E22+Materials!B22</f>
-        <v>57.194000000000003</v>
+        <v>35.989999999999995</v>
       </c>
       <c r="M22" s="5">
         <f t="shared" si="0"/>
-        <v>285.97000000000003</v>
+        <v>179.95</v>
       </c>
       <c r="N22" s="5">
         <f t="shared" si="1"/>
-        <v>236980.00000000003</v>
+        <v>95160</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
-      <c r="M23" s="5"/>
-      <c r="N23" s="5"/>
+      <c r="A23" s="2" t="str">
+        <f>Materials!A23</f>
+        <v>Copper-Hydride</v>
+      </c>
+      <c r="B23" s="6">
+        <f>((Materials!D23/2)+Materials!B23)</f>
+        <v>26.16</v>
+      </c>
+      <c r="C23" s="5">
+        <f>(Materials!G23/Materials!D23)+2</f>
+        <v>14.941176470588236</v>
+      </c>
+      <c r="D23" s="5">
+        <f>(Materials!B23*Materials!C23)+Materials!F23</f>
+        <v>165.345</v>
+      </c>
+      <c r="E23" s="5">
+        <f>(Materials!B23*Materials!C23)*Materials!D23</f>
+        <v>1538.7974999999999</v>
+      </c>
+      <c r="F23" s="5">
+        <f>((Materials!B23*Materials!C23)/2)+5</f>
+        <v>35.172499999999999</v>
+      </c>
+      <c r="G23" s="6">
+        <f>Materials!D23/Materials!C23</f>
+        <v>5.666666666666667</v>
+      </c>
+      <c r="H23" s="5">
+        <f>60+Materials!D23</f>
+        <v>85.5</v>
+      </c>
+      <c r="I23" s="6">
+        <f>Materials!G23/Materials!D23</f>
+        <v>12.941176470588236</v>
+      </c>
+      <c r="J23" s="5">
+        <f>Materials!G23*Materials!E23</f>
+        <v>2960.1000000000004</v>
+      </c>
+      <c r="K23" s="5">
+        <f>Materials!E23+Materials!C23</f>
+        <v>13.47</v>
+      </c>
+      <c r="L23" s="5">
+        <f>Materials!E23+Materials!B23</f>
+        <v>22.380000000000003</v>
+      </c>
+      <c r="M23" s="5">
+        <f t="shared" si="0"/>
+        <v>111.9</v>
+      </c>
+      <c r="N23" s="5">
+        <f t="shared" si="1"/>
+        <v>29601.000000000004</v>
+      </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
-      <c r="M24" s="5"/>
-      <c r="N24" s="5"/>
+      <c r="A24" s="2" t="str">
+        <f>Materials!A24</f>
+        <v>Stainless-Copilinvar-Tungstate</v>
+      </c>
+      <c r="B24" s="6">
+        <f>((Materials!D24/2)+Materials!B24)</f>
+        <v>187.03899999999999</v>
+      </c>
+      <c r="C24" s="5">
+        <f>(Materials!G24/Materials!D24)+2</f>
+        <v>12.701186623516721</v>
+      </c>
+      <c r="D24" s="5">
+        <f>(Materials!B24*Materials!C24)+Materials!F24</f>
+        <v>4244.3060000000005</v>
+      </c>
+      <c r="E24" s="5">
+        <f>(Materials!B24*Materials!C24)*Materials!D24</f>
+        <v>684428.6655</v>
+      </c>
+      <c r="F24" s="5">
+        <f>((Materials!B24*Materials!C24)/2)+5</f>
+        <v>1481.653</v>
+      </c>
+      <c r="G24" s="6">
+        <f>Materials!D24/Materials!C24</f>
+        <v>5.5843373493975905</v>
+      </c>
+      <c r="H24" s="5">
+        <f>60+Materials!D24</f>
+        <v>291.75</v>
+      </c>
+      <c r="I24" s="6">
+        <f>Materials!G24/Materials!D24</f>
+        <v>10.701186623516721</v>
+      </c>
+      <c r="J24" s="5">
+        <f>Materials!G24*Materials!E24</f>
+        <v>73631.199999999997</v>
+      </c>
+      <c r="K24" s="5">
+        <f>Materials!E24+Materials!C24</f>
+        <v>71.19</v>
+      </c>
+      <c r="L24" s="5">
+        <f>Materials!E24+Materials!B24</f>
+        <v>100.854</v>
+      </c>
+      <c r="M24" s="5">
+        <f t="shared" si="0"/>
+        <v>504.27</v>
+      </c>
+      <c r="N24" s="5">
+        <f t="shared" si="1"/>
+        <v>736312</v>
+      </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
@@ -2855,12 +2985,12 @@
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21:C22"/>
+      <selection activeCell="C22" sqref="C22:C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.28515625" style="4" bestFit="1" customWidth="1"/>
@@ -2889,7 +3019,7 @@
         <v>37</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
@@ -3206,15 +3336,15 @@
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="str">
         <f>Materials!A14</f>
-        <v>Cadmium</v>
+        <v>Zinc</v>
       </c>
       <c r="B14" s="6">
         <f>Materials!D14/2</f>
-        <v>2.2999999999999998</v>
+        <v>6</v>
       </c>
       <c r="C14" s="5">
         <f>Materials!G14+Materials!B14+Materials!C14+Materials!D14+Materials!E14</f>
-        <v>94.71</v>
+        <v>141.23999999999998</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
@@ -3256,15 +3386,15 @@
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="str">
         <f>Materials!A16</f>
-        <v>Stainless Steel</v>
+        <v>Aluminium</v>
       </c>
       <c r="B16" s="6">
         <f>Materials!D16/2</f>
-        <v>39.375</v>
+        <v>5</v>
       </c>
       <c r="C16" s="5">
         <f>Materials!G16+Materials!B16+Materials!C16+Materials!D16+Materials!E16</f>
-        <v>698.91099999999994</v>
+        <v>87.820000000000007</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
@@ -3281,15 +3411,15 @@
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="str">
         <f>Materials!A17</f>
-        <v>Bronze</v>
+        <v>Nickel</v>
       </c>
       <c r="B17" s="6">
         <f>Materials!D17/2</f>
-        <v>32</v>
+        <v>15.5</v>
       </c>
       <c r="C17" s="5">
         <f>Materials!G17+Materials!B17+Materials!C17+Materials!D17+Materials!E17</f>
-        <v>338.40000000000003</v>
+        <v>252.999</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
@@ -3306,15 +3436,15 @@
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="str">
         <f>Materials!A18</f>
-        <v>Elinvar</v>
+        <v>Stainless Steel</v>
       </c>
       <c r="B18" s="6">
         <f>Materials!D18/2</f>
-        <v>32.25</v>
+        <v>39.375</v>
       </c>
       <c r="C18" s="5">
         <f>Materials!G18+Materials!B18+Materials!C18+Materials!D18+Materials!E18</f>
-        <v>578.20400000000006</v>
+        <v>698.91099999999994</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
@@ -3331,15 +3461,15 @@
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="str">
         <f>Materials!A19</f>
-        <v>Billon</v>
+        <v>Bronze</v>
       </c>
       <c r="B19" s="6">
         <f>Materials!D19/2</f>
-        <v>13.75</v>
+        <v>32</v>
       </c>
       <c r="C19" s="5">
         <f>Materials!G19+Materials!B19+Materials!C19+Materials!D19+Materials!E19</f>
-        <v>644.95999999999992</v>
+        <v>338.40000000000003</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
@@ -3356,15 +3486,15 @@
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="str">
         <f>Materials!A20</f>
-        <v>Copper-Tungsten</v>
+        <v>Elinvar</v>
       </c>
       <c r="B20" s="6">
         <f>Materials!D20/2</f>
-        <v>28.75</v>
+        <v>47.75</v>
       </c>
       <c r="C20" s="5">
         <f>Materials!G20+Materials!B20+Materials!C20+Materials!D20+Materials!E20</f>
-        <v>1323.99</v>
+        <v>831.20299999999997</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
@@ -3381,15 +3511,15 @@
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="str">
         <f>Materials!A21</f>
-        <v>Copper-Hydride</v>
+        <v>Billon</v>
       </c>
       <c r="B21" s="6">
         <f>Materials!D21/2</f>
-        <v>12.75</v>
+        <v>13.75</v>
       </c>
       <c r="C21" s="5">
         <f>Materials!G21+Materials!B21+Materials!C21+Materials!D21+Materials!E21</f>
-        <v>382.38000000000005</v>
+        <v>644.95999999999992</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
@@ -3406,15 +3536,15 @@
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="str">
         <f>Materials!A22</f>
-        <v>Copilinvar-Tungstate</v>
+        <v>Copper-Tungsten</v>
       </c>
       <c r="B22" s="6">
         <f>Materials!D22/2</f>
-        <v>61</v>
+        <v>28.75</v>
       </c>
       <c r="C22" s="5">
         <f>Materials!G22+Materials!B22+Materials!C22+Materials!D22+Materials!E22</f>
-        <v>1902.194</v>
+        <v>1323.99</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
@@ -3429,9 +3559,18 @@
       <c r="N22" s="5"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="5"/>
+      <c r="A23" s="2" t="str">
+        <f>Materials!A23</f>
+        <v>Copper-Hydride</v>
+      </c>
+      <c r="B23" s="6">
+        <f>Materials!D23/2</f>
+        <v>12.75</v>
+      </c>
+      <c r="C23" s="5">
+        <f>Materials!G23+Materials!B23+Materials!C23+Materials!D23+Materials!E23</f>
+        <v>382.38000000000005</v>
+      </c>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
@@ -3445,9 +3584,18 @@
       <c r="N23" s="5"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="5"/>
+      <c r="A24" s="2" t="str">
+        <f>Materials!A24</f>
+        <v>Stainless-Copilinvar-Tungstate</v>
+      </c>
+      <c r="B24" s="6">
+        <f>Materials!D24/2</f>
+        <v>115.875</v>
+      </c>
+      <c r="C24" s="5">
+        <f>Materials!G24+Materials!B24+Materials!C24+Materials!D24+Materials!E24</f>
+        <v>2854.1040000000003</v>
+      </c>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>

</xml_diff>

<commit_message>
too many changes to count
</commit_message>
<xml_diff>
--- a/Info/balancing/metal system.xlsx
+++ b/Info/balancing/metal system.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>Density</t>
   </si>
@@ -165,6 +165,15 @@
   </si>
   <si>
     <t>Zinc</t>
+  </si>
+  <si>
+    <t>RGB: R</t>
+  </si>
+  <si>
+    <t>RGB: G</t>
+  </si>
+  <si>
+    <t>RGB: B</t>
   </si>
 </sst>
 </file>
@@ -605,7 +614,7 @@
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -622,7 +631,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -648,6 +657,15 @@
       </c>
       <c r="I1" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>50</v>
       </c>
       <c r="N1" t="s">
         <v>27</v>
@@ -681,6 +699,15 @@
       <c r="I2" s="3">
         <v>2862</v>
       </c>
+      <c r="J2" s="8">
+        <v>82</v>
+      </c>
+      <c r="K2" s="8">
+        <v>174</v>
+      </c>
+      <c r="L2" s="8">
+        <v>212</v>
+      </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -710,6 +737,15 @@
       <c r="I3" s="3">
         <v>2562</v>
       </c>
+      <c r="J3" s="8">
+        <v>212</v>
+      </c>
+      <c r="K3" s="8">
+        <v>119</v>
+      </c>
+      <c r="L3" s="8">
+        <v>82</v>
+      </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -745,6 +781,15 @@
       <c r="I4" s="3">
         <v>2862</v>
       </c>
+      <c r="J4" s="8">
+        <v>192</v>
+      </c>
+      <c r="K4" s="8">
+        <v>192</v>
+      </c>
+      <c r="L4" s="8">
+        <v>192</v>
+      </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -770,6 +815,15 @@
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
+      <c r="J5" s="8">
+        <v>182</v>
+      </c>
+      <c r="K5" s="8">
+        <v>155</v>
+      </c>
+      <c r="L5" s="8">
+        <v>76</v>
+      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -799,6 +853,15 @@
       <c r="I6" s="3">
         <v>5000</v>
       </c>
+      <c r="J6" s="8">
+        <v>139</v>
+      </c>
+      <c r="K6" s="8">
+        <v>141</v>
+      </c>
+      <c r="L6" s="8">
+        <v>122</v>
+      </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -828,6 +891,15 @@
       <c r="I7" s="3">
         <v>2670</v>
       </c>
+      <c r="J7" s="8">
+        <v>200</v>
+      </c>
+      <c r="K7" s="8">
+        <v>56</v>
+      </c>
+      <c r="L7" s="8">
+        <v>60</v>
+      </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -857,6 +929,15 @@
       <c r="I8" s="3">
         <v>2600</v>
       </c>
+      <c r="J8" s="8">
+        <v>39</v>
+      </c>
+      <c r="K8" s="8">
+        <v>105</v>
+      </c>
+      <c r="L8" s="8">
+        <v>135</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -886,6 +967,15 @@
       <c r="I9" s="3">
         <v>2212</v>
       </c>
+      <c r="J9" s="8">
+        <v>170</v>
+      </c>
+      <c r="K9" s="8">
+        <v>170</v>
+      </c>
+      <c r="L9" s="8">
+        <v>170</v>
+      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
@@ -915,6 +1005,15 @@
       <c r="I10" s="3">
         <v>2800</v>
       </c>
+      <c r="J10" s="8">
+        <v>134</v>
+      </c>
+      <c r="K10" s="8">
+        <v>128</v>
+      </c>
+      <c r="L10" s="8">
+        <v>34</v>
+      </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -944,6 +1043,15 @@
       <c r="I11" s="3">
         <v>1750</v>
       </c>
+      <c r="J11" s="8">
+        <v>105</v>
+      </c>
+      <c r="K11" s="8">
+        <v>213</v>
+      </c>
+      <c r="L11" s="8">
+        <v>212</v>
+      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
@@ -969,6 +1077,15 @@
       </c>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
+      <c r="J12" s="8">
+        <v>105</v>
+      </c>
+      <c r="K12" s="8">
+        <v>105</v>
+      </c>
+      <c r="L12" s="8">
+        <v>105</v>
+      </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
@@ -994,6 +1111,15 @@
       </c>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
+      <c r="J13" s="8">
+        <v>128</v>
+      </c>
+      <c r="K13" s="8">
+        <v>128</v>
+      </c>
+      <c r="L13" s="8">
+        <v>128</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
@@ -1023,6 +1149,15 @@
       <c r="I14" s="3">
         <v>907</v>
       </c>
+      <c r="J14" s="8">
+        <v>97</v>
+      </c>
+      <c r="K14" s="8">
+        <v>208</v>
+      </c>
+      <c r="L14" s="8">
+        <v>92</v>
+      </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
@@ -1052,6 +1187,15 @@
       <c r="I15" s="8">
         <v>5000</v>
       </c>
+      <c r="J15" s="8">
+        <v>87</v>
+      </c>
+      <c r="K15" s="8">
+        <v>87</v>
+      </c>
+      <c r="L15" s="8">
+        <v>87</v>
+      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
@@ -1081,8 +1225,17 @@
       <c r="I16" s="9">
         <v>2470</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16" s="8">
+        <v>150</v>
+      </c>
+      <c r="K16" s="8">
+        <v>150</v>
+      </c>
+      <c r="L16" s="8">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>46</v>
       </c>
@@ -1110,8 +1263,17 @@
       <c r="I17" s="8">
         <v>2730</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17" s="8">
+        <v>92</v>
+      </c>
+      <c r="K17" s="8">
+        <v>114</v>
+      </c>
+      <c r="L17" s="8">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>11</v>
       </c>
@@ -1147,8 +1309,20 @@
         <f>AVERAGE(I4,I7)</f>
         <v>2766</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18" s="8">
+        <f t="shared" ref="J18:L18" si="2">AVERAGE(J4,J7)</f>
+        <v>196</v>
+      </c>
+      <c r="K18" s="8">
+        <f t="shared" si="2"/>
+        <v>124</v>
+      </c>
+      <c r="L18" s="8">
+        <f t="shared" si="2"/>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>28</v>
       </c>
@@ -1157,23 +1331,23 @@
         <v>16.22</v>
       </c>
       <c r="C19" s="9">
-        <f t="shared" ref="C19:G19" si="2">C3+C8</f>
+        <f t="shared" ref="C19:G19" si="3">C3+C8</f>
         <v>4.5</v>
       </c>
       <c r="D19" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>64</v>
       </c>
       <c r="E19" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>14.68</v>
       </c>
       <c r="F19" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>79</v>
       </c>
       <c r="G19" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>239</v>
       </c>
       <c r="H19" s="8">
@@ -1184,8 +1358,20 @@
         <f>AVERAGE(I3,I8)</f>
         <v>2581</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J19" s="8">
+        <f t="shared" ref="J19:L19" si="4">AVERAGE(J3,J8)</f>
+        <v>125.5</v>
+      </c>
+      <c r="K19" s="8">
+        <f t="shared" si="4"/>
+        <v>112</v>
+      </c>
+      <c r="L19" s="8">
+        <f t="shared" si="4"/>
+        <v>108.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>41</v>
       </c>
@@ -1194,23 +1380,23 @@
         <v>23.972999999999999</v>
       </c>
       <c r="C20" s="9">
-        <f t="shared" ref="C20:G20" si="3">C2+C7+C17</f>
+        <f t="shared" ref="C20:G20" si="5">C2+C7+C17</f>
         <v>16.5</v>
       </c>
       <c r="D20" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>95.5</v>
       </c>
       <c r="E20" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>15.23</v>
       </c>
       <c r="F20" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>366</v>
       </c>
       <c r="G20" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>680</v>
       </c>
       <c r="H20" s="8">
@@ -1221,8 +1407,20 @@
         <f>AVERAGE(I17,I7,I2)</f>
         <v>2754</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J20" s="8">
+        <f t="shared" ref="J20:L20" si="6">AVERAGE(J17,J7,J2)</f>
+        <v>124.66666666666667</v>
+      </c>
+      <c r="K20" s="8">
+        <f t="shared" si="6"/>
+        <v>114.66666666666667</v>
+      </c>
+      <c r="L20" s="8">
+        <f t="shared" si="6"/>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>42</v>
       </c>
@@ -1231,23 +1429,23 @@
         <v>19.43</v>
       </c>
       <c r="C21" s="3">
-        <f t="shared" ref="C21:G21" si="4">C3+C9</f>
+        <f t="shared" ref="C21:G21" si="7">C3+C9</f>
         <v>5.75</v>
       </c>
       <c r="D21" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>27.5</v>
       </c>
       <c r="E21" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>12.280000000000001</v>
       </c>
       <c r="F21" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>125</v>
       </c>
       <c r="G21" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>580</v>
       </c>
       <c r="H21" s="3">
@@ -1258,8 +1456,20 @@
         <f>AVERAGE(I3,I9)</f>
         <v>2387</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J21" s="8">
+        <f t="shared" ref="J21:L21" si="8">AVERAGE(J3,J9)</f>
+        <v>191</v>
+      </c>
+      <c r="K21" s="8">
+        <f t="shared" si="8"/>
+        <v>144.5</v>
+      </c>
+      <c r="L21" s="8">
+        <f t="shared" si="8"/>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>39</v>
       </c>
@@ -1268,23 +1478,23 @@
         <v>28.189999999999998</v>
       </c>
       <c r="C22" s="9">
-        <f t="shared" ref="C22:G22" si="5">C15+C3</f>
+        <f t="shared" ref="C22:G22" si="9">C15+C3</f>
         <v>10.5</v>
       </c>
       <c r="D22" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>57.5</v>
       </c>
       <c r="E22" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>7.8000000000000007</v>
       </c>
       <c r="F22" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>570</v>
       </c>
       <c r="G22" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>1220</v>
       </c>
       <c r="H22" s="8">
@@ -1295,8 +1505,20 @@
         <f>AVERAGE(I17,I5)</f>
         <v>2730</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J22" s="8">
+        <f t="shared" ref="J22:L22" si="10">AVERAGE(J17,J5)</f>
+        <v>137</v>
+      </c>
+      <c r="K22" s="8">
+        <f t="shared" si="10"/>
+        <v>134.5</v>
+      </c>
+      <c r="L22" s="8">
+        <f t="shared" si="10"/>
+        <v>142</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>40</v>
       </c>
@@ -1305,35 +1527,47 @@
         <v>13.41</v>
       </c>
       <c r="C23" s="3">
-        <f t="shared" ref="C23:I23" si="6">(C3*2)*0.75</f>
+        <f t="shared" ref="C23:L23" si="11">(C3*2)*0.75</f>
         <v>4.5</v>
       </c>
       <c r="D23" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>25.5</v>
       </c>
       <c r="E23" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>8.9700000000000006</v>
       </c>
       <c r="F23" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>105</v>
       </c>
       <c r="G23" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>330</v>
       </c>
       <c r="H23" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>1626</v>
       </c>
       <c r="I23" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>3843</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J23" s="8">
+        <f>(J3*2)*0.5</f>
+        <v>212</v>
+      </c>
+      <c r="K23" s="8">
+        <f t="shared" si="11"/>
+        <v>178.5</v>
+      </c>
+      <c r="L23" s="8">
+        <f t="shared" si="11"/>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>44</v>
       </c>
@@ -1342,23 +1576,23 @@
         <v>71.164000000000001</v>
       </c>
       <c r="C24" s="9">
-        <f t="shared" ref="C24:I24" si="7">C18+C20+C22</f>
+        <f t="shared" ref="C24:G24" si="12">C18+C20+C22</f>
         <v>41.5</v>
       </c>
       <c r="D24" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>231.75</v>
       </c>
       <c r="E24" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>29.69</v>
       </c>
       <c r="F24" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>1291</v>
       </c>
       <c r="G24" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>2480</v>
       </c>
       <c r="H24" s="8">
@@ -1369,8 +1603,20 @@
         <f>AVERAGE(I18,I20,I22)</f>
         <v>2750</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J24" s="8">
+        <f t="shared" ref="J24:L24" si="13">AVERAGE(J18,J20,J22)</f>
+        <v>152.55555555555557</v>
+      </c>
+      <c r="K24" s="8">
+        <f t="shared" si="13"/>
+        <v>124.3888888888889</v>
+      </c>
+      <c r="L24" s="8">
+        <f t="shared" si="13"/>
+        <v>142.66666666666666</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1380,8 +1626,11 @@
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1391,8 +1640,11 @@
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -1402,8 +1654,11 @@
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -1413,8 +1668,11 @@
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -1424,8 +1682,11 @@
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -1435,8 +1696,11 @@
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -1446,6 +1710,9 @@
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>